<commit_message>
Speed up column placement more
</commit_message>
<xml_diff>
--- a/Test Results.xlsx
+++ b/Test Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Documents\RevitUtilities-master\RevitUtilities-master\Column Sort - Current\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D90ADBAE-B542-4AEB-B074-A326827926C7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0F955D-DEDB-423E-A4E8-B957EFC40917}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6784F4F-6013-4AC1-BB34-1B8804D31140}"/>
+    <workbookView xWindow="4530" yWindow="1950" windowWidth="11820" windowHeight="10710" xr2:uid="{B6784F4F-6013-4AC1-BB34-1B8804D31140}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="101">
   <si>
     <t>Start</t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>Get results for child 24</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -338,7 +341,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -371,7 +374,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -687,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B55F16F4-02C8-43F7-AF82-ACA786E304B0}">
-  <dimension ref="C1:Q112"/>
+  <dimension ref="C1:Q122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="D119" sqref="D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1644,6 +1647,26 @@
         <f>H27-H26</f>
         <v>0</v>
       </c>
+      <c r="K27" t="s">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27" s="2">
+        <f t="shared" ref="M27:M57" si="4">L27-L26</f>
+        <v>0</v>
+      </c>
+      <c r="O27" t="s">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="2">
+        <f t="shared" ref="Q27:Q57" si="5">P27-P26</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
@@ -1666,6 +1689,26 @@
         <f>H28-H27</f>
         <v>1.3782363</v>
       </c>
+      <c r="K28" t="s">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>1.2533565</v>
+      </c>
+      <c r="M28" s="2">
+        <f t="shared" si="4"/>
+        <v>1.2533565</v>
+      </c>
+      <c r="O28" t="s">
+        <v>1</v>
+      </c>
+      <c r="P28">
+        <v>1.3127005</v>
+      </c>
+      <c r="Q28" s="2">
+        <f t="shared" si="5"/>
+        <v>1.3127005</v>
+      </c>
     </row>
     <row r="29" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
@@ -1675,7 +1718,7 @@
         <v>4.6610586999999999</v>
       </c>
       <c r="E29" s="2">
-        <f t="shared" ref="E29:E92" si="4">D29-D28</f>
+        <f t="shared" ref="E29:E92" si="6">D29-D28</f>
         <v>2.8551757999999996</v>
       </c>
       <c r="G29" t="s">
@@ -1685,8 +1728,28 @@
         <v>3.6015972000000001</v>
       </c>
       <c r="I29" s="2">
-        <f t="shared" ref="I29:I92" si="5">H29-H28</f>
+        <f t="shared" ref="I29:I92" si="7">H29-H28</f>
         <v>2.2233609000000003</v>
+      </c>
+      <c r="K29" t="s">
+        <v>24</v>
+      </c>
+      <c r="L29">
+        <v>3.3080609000000001</v>
+      </c>
+      <c r="M29" s="2">
+        <f t="shared" si="4"/>
+        <v>2.0547044000000003</v>
+      </c>
+      <c r="O29" t="s">
+        <v>24</v>
+      </c>
+      <c r="P29">
+        <v>3.5316724000000002</v>
+      </c>
+      <c r="Q29" s="2">
+        <f t="shared" si="5"/>
+        <v>2.2189719000000001</v>
       </c>
     </row>
     <row r="30" spans="3:17" x14ac:dyDescent="0.25">
@@ -1697,7 +1760,7 @@
         <v>15.635734899999999</v>
       </c>
       <c r="E30" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10.974676199999999</v>
       </c>
       <c r="G30" t="s">
@@ -1707,8 +1770,28 @@
         <v>9.5964495999999997</v>
       </c>
       <c r="I30" s="2">
+        <f t="shared" si="7"/>
+        <v>5.9948523999999992</v>
+      </c>
+      <c r="K30" t="s">
+        <v>25</v>
+      </c>
+      <c r="L30">
+        <v>9.7067616999999995</v>
+      </c>
+      <c r="M30" s="2">
+        <f t="shared" si="4"/>
+        <v>6.3987007999999994</v>
+      </c>
+      <c r="O30" t="s">
+        <v>25</v>
+      </c>
+      <c r="P30">
+        <v>9.8052857000000007</v>
+      </c>
+      <c r="Q30" s="2">
         <f t="shared" si="5"/>
-        <v>5.9948523999999992</v>
+        <v>6.2736133000000009</v>
       </c>
     </row>
     <row r="31" spans="3:17" x14ac:dyDescent="0.25">
@@ -1719,7 +1802,7 @@
         <v>20.290229799999999</v>
       </c>
       <c r="E31" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.6544948999999995</v>
       </c>
       <c r="G31" t="s">
@@ -1729,8 +1812,28 @@
         <v>13.211523700000001</v>
       </c>
       <c r="I31" s="2">
+        <f t="shared" si="7"/>
+        <v>3.6150741000000011</v>
+      </c>
+      <c r="K31" t="s">
+        <v>26</v>
+      </c>
+      <c r="L31">
+        <v>13.2862651</v>
+      </c>
+      <c r="M31" s="2">
+        <f t="shared" si="4"/>
+        <v>3.5795034000000001</v>
+      </c>
+      <c r="O31" t="s">
+        <v>26</v>
+      </c>
+      <c r="P31">
+        <v>13.4423447</v>
+      </c>
+      <c r="Q31" s="2">
         <f t="shared" si="5"/>
-        <v>3.6150741000000011</v>
+        <v>3.6370589999999989</v>
       </c>
     </row>
     <row r="32" spans="3:17" x14ac:dyDescent="0.25">
@@ -1741,7 +1844,7 @@
         <v>20.302172599999999</v>
       </c>
       <c r="E32" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.194279999999992E-2</v>
       </c>
       <c r="G32" t="s">
@@ -1751,11 +1854,31 @@
         <v>13.220488700000001</v>
       </c>
       <c r="I32" s="2">
+        <f t="shared" si="7"/>
+        <v>8.9649999999998897E-3</v>
+      </c>
+      <c r="K32" t="s">
+        <v>27</v>
+      </c>
+      <c r="L32">
+        <v>13.294270600000001</v>
+      </c>
+      <c r="M32" s="2">
+        <f t="shared" si="4"/>
+        <v>8.00550000000122E-3</v>
+      </c>
+      <c r="O32" t="s">
+        <v>27</v>
+      </c>
+      <c r="P32">
+        <v>13.451294799999999</v>
+      </c>
+      <c r="Q32" s="2">
         <f t="shared" si="5"/>
-        <v>8.9649999999998897E-3</v>
-      </c>
-    </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+        <v>8.9500999999998498E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>28</v>
       </c>
@@ -1763,7 +1886,7 @@
         <v>20.3061881</v>
       </c>
       <c r="E33" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.0155000000012819E-3</v>
       </c>
       <c r="G33" t="s">
@@ -1773,11 +1896,31 @@
         <v>13.222467</v>
       </c>
       <c r="I33" s="2">
+        <f t="shared" si="7"/>
+        <v>1.9782999999993223E-3</v>
+      </c>
+      <c r="K33" t="s">
+        <v>28</v>
+      </c>
+      <c r="L33">
+        <v>13.2972638</v>
+      </c>
+      <c r="M33" s="2">
+        <f t="shared" si="4"/>
+        <v>2.9931999999988079E-3</v>
+      </c>
+      <c r="O33" t="s">
+        <v>28</v>
+      </c>
+      <c r="P33">
+        <v>13.454306300000001</v>
+      </c>
+      <c r="Q33" s="2">
         <f t="shared" si="5"/>
-        <v>1.9782999999993223E-3</v>
-      </c>
-    </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+        <v>3.011500000001277E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>29</v>
       </c>
@@ -1785,7 +1928,7 @@
         <v>20.308157099999999</v>
       </c>
       <c r="E34" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.9689999999989993E-3</v>
       </c>
       <c r="G34" t="s">
@@ -1795,11 +1938,31 @@
         <v>13.224487</v>
       </c>
       <c r="I34" s="2">
+        <f t="shared" si="7"/>
+        <v>2.0199999999999108E-3</v>
+      </c>
+      <c r="K34" t="s">
+        <v>29</v>
+      </c>
+      <c r="L34">
+        <v>13.2992563</v>
+      </c>
+      <c r="M34" s="2">
+        <f t="shared" si="4"/>
+        <v>1.9925000000000637E-3</v>
+      </c>
+      <c r="O34" t="s">
+        <v>29</v>
+      </c>
+      <c r="P34">
+        <v>13.456306400000001</v>
+      </c>
+      <c r="Q34" s="2">
         <f t="shared" si="5"/>
-        <v>2.0199999999999108E-3</v>
-      </c>
-    </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+        <v>2.0001000000000602E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>30</v>
       </c>
@@ -1807,7 +1970,7 @@
         <v>20.313169299999998</v>
       </c>
       <c r="E35" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.0121999999994671E-3</v>
       </c>
       <c r="G35" t="s">
@@ -1817,11 +1980,31 @@
         <v>13.22845</v>
       </c>
       <c r="I35" s="2">
+        <f t="shared" si="7"/>
+        <v>3.9630000000006049E-3</v>
+      </c>
+      <c r="K35" t="s">
+        <v>30</v>
+      </c>
+      <c r="L35">
+        <v>13.303244400000001</v>
+      </c>
+      <c r="M35" s="2">
+        <f t="shared" si="4"/>
+        <v>3.9881000000008271E-3</v>
+      </c>
+      <c r="O35" t="s">
+        <v>30</v>
+      </c>
+      <c r="P35">
+        <v>13.460270400000001</v>
+      </c>
+      <c r="Q35" s="2">
         <f t="shared" si="5"/>
-        <v>3.9630000000006049E-3</v>
-      </c>
-    </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+        <v>3.9639999999998565E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>31</v>
       </c>
@@ -1829,7 +2012,7 @@
         <v>20.3151388</v>
       </c>
       <c r="E36" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.9695000000012897E-3</v>
       </c>
       <c r="G36" t="s">
@@ -1839,11 +2022,31 @@
         <v>13.2304449</v>
       </c>
       <c r="I36" s="2">
+        <f t="shared" si="7"/>
+        <v>1.9948999999996886E-3</v>
+      </c>
+      <c r="K36" t="s">
+        <v>31</v>
+      </c>
+      <c r="L36">
+        <v>13.3052405</v>
+      </c>
+      <c r="M36" s="2">
+        <f t="shared" si="4"/>
+        <v>1.9960999999995011E-3</v>
+      </c>
+      <c r="O36" t="s">
+        <v>31</v>
+      </c>
+      <c r="P36">
+        <v>13.463292900000001</v>
+      </c>
+      <c r="Q36" s="2">
         <f t="shared" si="5"/>
-        <v>1.9948999999996886E-3</v>
-      </c>
-    </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
+        <v>3.0225000000001501E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>37</v>
       </c>
@@ -1851,7 +2054,7 @@
         <v>20.3171331</v>
       </c>
       <c r="E37" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.9942999999997824E-3</v>
       </c>
       <c r="G37" t="s">
@@ -1861,11 +2064,31 @@
         <v>13.2334365</v>
       </c>
       <c r="I37" s="2">
+        <f t="shared" si="7"/>
+        <v>2.9915999999996501E-3</v>
+      </c>
+      <c r="K37" t="s">
+        <v>37</v>
+      </c>
+      <c r="L37">
+        <v>13.308206999999999</v>
+      </c>
+      <c r="M37" s="2">
+        <f t="shared" si="4"/>
+        <v>2.9664999999994279E-3</v>
+      </c>
+      <c r="O37" t="s">
+        <v>37</v>
+      </c>
+      <c r="P37">
+        <v>13.4652823</v>
+      </c>
+      <c r="Q37" s="2">
         <f t="shared" si="5"/>
-        <v>2.9915999999996501E-3</v>
-      </c>
-    </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
+        <v>1.9893999999993639E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>38</v>
       </c>
@@ -1873,7 +2096,7 @@
         <v>20.320125000000001</v>
       </c>
       <c r="E38" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.9919000000013796E-3</v>
       </c>
       <c r="G38" t="s">
@@ -1883,11 +2106,31 @@
         <v>13.235431200000001</v>
       </c>
       <c r="I38" s="2">
+        <f t="shared" si="7"/>
+        <v>1.9947000000009041E-3</v>
+      </c>
+      <c r="K38" t="s">
+        <v>38</v>
+      </c>
+      <c r="L38">
+        <v>13.3102257</v>
+      </c>
+      <c r="M38" s="2">
+        <f t="shared" si="4"/>
+        <v>2.018700000000706E-3</v>
+      </c>
+      <c r="O38" t="s">
+        <v>38</v>
+      </c>
+      <c r="P38">
+        <v>13.4672523</v>
+      </c>
+      <c r="Q38" s="2">
         <f t="shared" si="5"/>
-        <v>1.9947000000009041E-3</v>
-      </c>
-    </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
+        <v>1.9700000000000273E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>39</v>
       </c>
@@ -1895,7 +2138,7 @@
         <v>20.323143099999999</v>
       </c>
       <c r="E39" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.0180999999984692E-3</v>
       </c>
       <c r="G39" t="s">
@@ -1905,11 +2148,31 @@
         <v>13.237425999999999</v>
       </c>
       <c r="I39" s="2">
+        <f t="shared" si="7"/>
+        <v>1.99479999999852E-3</v>
+      </c>
+      <c r="K39" t="s">
+        <v>39</v>
+      </c>
+      <c r="L39">
+        <v>13.312220399999999</v>
+      </c>
+      <c r="M39" s="2">
+        <f t="shared" si="4"/>
+        <v>1.9946999999991277E-3</v>
+      </c>
+      <c r="O39" t="s">
+        <v>39</v>
+      </c>
+      <c r="P39">
+        <v>13.4692718</v>
+      </c>
+      <c r="Q39" s="2">
         <f t="shared" si="5"/>
-        <v>1.99479999999852E-3</v>
-      </c>
-    </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
+        <v>2.0194999999993968E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>40</v>
       </c>
@@ -1917,7 +2180,7 @@
         <v>20.326136900000002</v>
       </c>
       <c r="E40" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.9938000000022669E-3</v>
       </c>
       <c r="G40" t="s">
@@ -1927,11 +2190,31 @@
         <v>13.240445100000001</v>
       </c>
       <c r="I40" s="2">
+        <f t="shared" si="7"/>
+        <v>3.0191000000012735E-3</v>
+      </c>
+      <c r="K40" t="s">
+        <v>40</v>
+      </c>
+      <c r="L40">
+        <v>13.3142152</v>
+      </c>
+      <c r="M40" s="2">
+        <f t="shared" si="4"/>
+        <v>1.9948000000002963E-3</v>
+      </c>
+      <c r="O40" t="s">
+        <v>40</v>
+      </c>
+      <c r="P40">
+        <v>13.471265600000001</v>
+      </c>
+      <c r="Q40" s="2">
         <f t="shared" si="5"/>
-        <v>3.0191000000012735E-3</v>
-      </c>
-    </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
+        <v>1.9938000000010447E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>41</v>
       </c>
@@ -1939,7 +2222,7 @@
         <v>20.328103500000001</v>
       </c>
       <c r="E41" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.9665999999993744E-3</v>
       </c>
       <c r="G41" t="s">
@@ -1949,11 +2232,31 @@
         <v>13.2424132</v>
       </c>
       <c r="I41" s="2">
+        <f t="shared" si="7"/>
+        <v>1.96809999999914E-3</v>
+      </c>
+      <c r="K41" t="s">
+        <v>41</v>
+      </c>
+      <c r="L41">
+        <v>13.3172084</v>
+      </c>
+      <c r="M41" s="2">
+        <f t="shared" si="4"/>
+        <v>2.9932000000005843E-3</v>
+      </c>
+      <c r="O41" t="s">
+        <v>41</v>
+      </c>
+      <c r="P41">
+        <v>13.4742336</v>
+      </c>
+      <c r="Q41" s="2">
         <f t="shared" si="5"/>
-        <v>1.96809999999914E-3</v>
-      </c>
-    </row>
-    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
+        <v>2.9679999999991935E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>42</v>
       </c>
@@ -1961,7 +2264,7 @@
         <v>20.330128200000001</v>
       </c>
       <c r="E42" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.0246999999997684E-3</v>
       </c>
       <c r="G42" t="s">
@@ -1971,187 +2274,367 @@
         <v>13.244434699999999</v>
       </c>
       <c r="I42" s="2">
+        <f t="shared" si="7"/>
+        <v>2.0214999999996763E-3</v>
+      </c>
+      <c r="K42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L42">
+        <v>13.3192042</v>
+      </c>
+      <c r="M42" s="2">
+        <f t="shared" si="4"/>
+        <v>1.9957999999995479E-3</v>
+      </c>
+      <c r="O42" t="s">
+        <v>42</v>
+      </c>
+      <c r="P42">
+        <v>13.476252199999999</v>
+      </c>
+      <c r="Q42" s="2">
+        <f t="shared" si="5"/>
+        <v>2.0185999999995374E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>43</v>
+      </c>
+      <c r="D43">
+        <v>20.333090299999999</v>
+      </c>
+      <c r="E43" s="2">
+        <f t="shared" si="6"/>
+        <v>2.9620999999977471E-3</v>
+      </c>
+      <c r="G43" t="s">
+        <v>43</v>
+      </c>
+      <c r="H43">
+        <v>13.2474259</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" si="7"/>
+        <v>2.9912000000003047E-3</v>
+      </c>
+      <c r="K43" t="s">
+        <v>43</v>
+      </c>
+      <c r="L43">
+        <v>13.321235</v>
+      </c>
+      <c r="M43" s="2">
+        <f t="shared" si="4"/>
+        <v>2.0307999999999993E-3</v>
+      </c>
+      <c r="O43" t="s">
+        <v>43</v>
+      </c>
+      <c r="P43">
+        <v>13.4782475</v>
+      </c>
+      <c r="Q43" s="2">
+        <f t="shared" si="5"/>
+        <v>1.9953000000008103E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44">
+        <v>20.337107100000001</v>
+      </c>
+      <c r="E44" s="2">
+        <f t="shared" si="6"/>
+        <v>4.016800000002263E-3</v>
+      </c>
+      <c r="G44" t="s">
+        <v>44</v>
+      </c>
+      <c r="H44">
+        <v>13.2503917</v>
+      </c>
+      <c r="I44" s="2">
+        <f t="shared" si="7"/>
+        <v>2.9658000000001294E-3</v>
+      </c>
+      <c r="K44" t="s">
+        <v>44</v>
+      </c>
+      <c r="L44">
+        <v>13.3251948</v>
+      </c>
+      <c r="M44" s="2">
+        <f t="shared" si="4"/>
+        <v>3.9598000000005129E-3</v>
+      </c>
+      <c r="O44" t="s">
+        <v>44</v>
+      </c>
+      <c r="P44">
+        <v>13.482237100000001</v>
+      </c>
+      <c r="Q44" s="2">
+        <f t="shared" si="5"/>
+        <v>3.9896000000005927E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>45</v>
+      </c>
+      <c r="D45">
+        <v>20.341095599999999</v>
+      </c>
+      <c r="E45" s="2">
+        <f t="shared" si="6"/>
+        <v>3.9884999999983961E-3</v>
+      </c>
+      <c r="G45" t="s">
+        <v>45</v>
+      </c>
+      <c r="H45">
+        <v>13.2534109</v>
+      </c>
+      <c r="I45" s="2">
+        <f t="shared" si="7"/>
+        <v>3.0192000000006658E-3</v>
+      </c>
+      <c r="K45" t="s">
+        <v>45</v>
+      </c>
+      <c r="L45">
+        <v>13.328206700000001</v>
+      </c>
+      <c r="M45" s="2">
+        <f t="shared" si="4"/>
+        <v>3.0119000000006224E-3</v>
+      </c>
+      <c r="O45" t="s">
+        <v>45</v>
+      </c>
+      <c r="P45">
+        <v>13.4852297</v>
+      </c>
+      <c r="Q45" s="2">
+        <f t="shared" si="5"/>
+        <v>2.9925999999989017E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D46">
+        <v>20.343063600000001</v>
+      </c>
+      <c r="E46" s="2">
+        <f t="shared" si="6"/>
+        <v>1.9680000000015241E-3</v>
+      </c>
+      <c r="G46" t="s">
+        <v>46</v>
+      </c>
+      <c r="H46">
+        <v>13.255403299999999</v>
+      </c>
+      <c r="I46" s="2">
+        <f t="shared" si="7"/>
+        <v>1.9923999999988951E-3</v>
+      </c>
+      <c r="K46" t="s">
+        <v>46</v>
+      </c>
+      <c r="L46">
+        <v>13.330205599999999</v>
+      </c>
+      <c r="M46" s="2">
+        <f t="shared" si="4"/>
+        <v>1.9988999999984713E-3</v>
+      </c>
+      <c r="O46" t="s">
+        <v>46</v>
+      </c>
+      <c r="P46">
+        <v>13.488195299999999</v>
+      </c>
+      <c r="Q46" s="2">
+        <f t="shared" si="5"/>
+        <v>2.9655999999995686E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>47</v>
+      </c>
+      <c r="D47">
+        <v>20.346083700000001</v>
+      </c>
+      <c r="E47" s="2">
+        <f t="shared" si="6"/>
+        <v>3.0201000000005251E-3</v>
+      </c>
+      <c r="G47" t="s">
+        <v>47</v>
+      </c>
+      <c r="H47">
+        <v>13.259392500000001</v>
+      </c>
+      <c r="I47" s="2">
+        <f t="shared" si="7"/>
+        <v>3.9892000000012473E-3</v>
+      </c>
+      <c r="K47" t="s">
+        <v>47</v>
+      </c>
+      <c r="L47">
+        <v>13.3322007</v>
+      </c>
+      <c r="M47" s="2">
+        <f t="shared" si="4"/>
+        <v>1.9951000000002495E-3</v>
+      </c>
+      <c r="O47" t="s">
+        <v>47</v>
+      </c>
+      <c r="P47">
+        <v>13.4911885</v>
+      </c>
+      <c r="Q47" s="2">
+        <f t="shared" si="5"/>
+        <v>2.9932000000005843E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48">
+        <v>20.3480749</v>
+      </c>
+      <c r="E48" s="2">
+        <f t="shared" si="6"/>
+        <v>1.9911999999990826E-3</v>
+      </c>
+      <c r="G48" t="s">
+        <v>48</v>
+      </c>
+      <c r="H48">
+        <v>13.261386999999999</v>
+      </c>
+      <c r="I48" s="2">
+        <f t="shared" si="7"/>
+        <v>1.9944999999985669E-3</v>
+      </c>
+      <c r="K48" t="s">
+        <v>48</v>
+      </c>
+      <c r="L48">
+        <v>13.3351922</v>
+      </c>
+      <c r="M48" s="2">
+        <f t="shared" si="4"/>
+        <v>2.9915000000002578E-3</v>
+      </c>
+      <c r="O48" t="s">
+        <v>48</v>
+      </c>
+      <c r="P48">
+        <v>13.4931828</v>
+      </c>
+      <c r="Q48" s="2">
+        <f t="shared" si="5"/>
+        <v>1.9942999999997824E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49">
+        <v>20.3500692</v>
+      </c>
+      <c r="E49" s="2">
+        <f t="shared" si="6"/>
+        <v>1.9942999999997824E-3</v>
+      </c>
+      <c r="G49" t="s">
+        <v>49</v>
+      </c>
+      <c r="H49">
+        <v>13.263381499999999</v>
+      </c>
+      <c r="I49" s="2">
+        <f t="shared" si="7"/>
+        <v>1.9945000000003432E-3</v>
+      </c>
+      <c r="K49" t="s">
+        <v>49</v>
+      </c>
+      <c r="L49">
+        <v>13.337187</v>
+      </c>
+      <c r="M49" s="2">
+        <f t="shared" si="4"/>
+        <v>1.9948000000002963E-3</v>
+      </c>
+      <c r="O49" t="s">
+        <v>49</v>
+      </c>
+      <c r="P49">
+        <v>13.496173900000001</v>
+      </c>
+      <c r="Q49" s="2">
+        <f t="shared" si="5"/>
+        <v>2.9911000000009125E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>50</v>
+      </c>
+      <c r="D50">
+        <v>20.354033999999999</v>
+      </c>
+      <c r="E50" s="2">
+        <f t="shared" si="6"/>
+        <v>3.9647999999985473E-3</v>
+      </c>
+      <c r="G50" t="s">
+        <v>50</v>
+      </c>
+      <c r="H50">
+        <v>13.266348499999999</v>
+      </c>
+      <c r="I50" s="2">
+        <f t="shared" si="7"/>
+        <v>2.9669999999999419E-3</v>
+      </c>
+      <c r="K50" t="s">
+        <v>50</v>
+      </c>
+      <c r="L50">
+        <v>13.340180500000001</v>
+      </c>
+      <c r="M50" s="2">
+        <f t="shared" si="4"/>
+        <v>2.9935000000005374E-3</v>
+      </c>
+      <c r="O50" t="s">
+        <v>50</v>
+      </c>
+      <c r="P50">
+        <v>13.4981954</v>
+      </c>
+      <c r="Q50" s="2">
         <f t="shared" si="5"/>
         <v>2.0214999999996763E-3</v>
       </c>
     </row>
-    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>43</v>
-      </c>
-      <c r="D43">
-        <v>20.333090299999999</v>
-      </c>
-      <c r="E43" s="2">
-        <f t="shared" si="4"/>
-        <v>2.9620999999977471E-3</v>
-      </c>
-      <c r="G43" t="s">
-        <v>43</v>
-      </c>
-      <c r="H43">
-        <v>13.2474259</v>
-      </c>
-      <c r="I43" s="2">
-        <f t="shared" si="5"/>
-        <v>2.9912000000003047E-3</v>
-      </c>
-    </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>44</v>
-      </c>
-      <c r="D44">
-        <v>20.337107100000001</v>
-      </c>
-      <c r="E44" s="2">
-        <f t="shared" si="4"/>
-        <v>4.016800000002263E-3</v>
-      </c>
-      <c r="G44" t="s">
-        <v>44</v>
-      </c>
-      <c r="H44">
-        <v>13.2503917</v>
-      </c>
-      <c r="I44" s="2">
-        <f t="shared" si="5"/>
-        <v>2.9658000000001294E-3</v>
-      </c>
-    </row>
-    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>45</v>
-      </c>
-      <c r="D45">
-        <v>20.341095599999999</v>
-      </c>
-      <c r="E45" s="2">
-        <f t="shared" si="4"/>
-        <v>3.9884999999983961E-3</v>
-      </c>
-      <c r="G45" t="s">
-        <v>45</v>
-      </c>
-      <c r="H45">
-        <v>13.2534109</v>
-      </c>
-      <c r="I45" s="2">
-        <f t="shared" si="5"/>
-        <v>3.0192000000006658E-3</v>
-      </c>
-    </row>
-    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>46</v>
-      </c>
-      <c r="D46">
-        <v>20.343063600000001</v>
-      </c>
-      <c r="E46" s="2">
-        <f t="shared" si="4"/>
-        <v>1.9680000000015241E-3</v>
-      </c>
-      <c r="G46" t="s">
-        <v>46</v>
-      </c>
-      <c r="H46">
-        <v>13.255403299999999</v>
-      </c>
-      <c r="I46" s="2">
-        <f t="shared" si="5"/>
-        <v>1.9923999999988951E-3</v>
-      </c>
-    </row>
-    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
-        <v>47</v>
-      </c>
-      <c r="D47">
-        <v>20.346083700000001</v>
-      </c>
-      <c r="E47" s="2">
-        <f t="shared" si="4"/>
-        <v>3.0201000000005251E-3</v>
-      </c>
-      <c r="G47" t="s">
-        <v>47</v>
-      </c>
-      <c r="H47">
-        <v>13.259392500000001</v>
-      </c>
-      <c r="I47" s="2">
-        <f t="shared" si="5"/>
-        <v>3.9892000000012473E-3</v>
-      </c>
-    </row>
-    <row r="48" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
-        <v>48</v>
-      </c>
-      <c r="D48">
-        <v>20.3480749</v>
-      </c>
-      <c r="E48" s="2">
-        <f t="shared" si="4"/>
-        <v>1.9911999999990826E-3</v>
-      </c>
-      <c r="G48" t="s">
-        <v>48</v>
-      </c>
-      <c r="H48">
-        <v>13.261386999999999</v>
-      </c>
-      <c r="I48" s="2">
-        <f t="shared" si="5"/>
-        <v>1.9944999999985669E-3</v>
-      </c>
-    </row>
-    <row r="49" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
-        <v>49</v>
-      </c>
-      <c r="D49">
-        <v>20.3500692</v>
-      </c>
-      <c r="E49" s="2">
-        <f t="shared" si="4"/>
-        <v>1.9942999999997824E-3</v>
-      </c>
-      <c r="G49" t="s">
-        <v>49</v>
-      </c>
-      <c r="H49">
-        <v>13.263381499999999</v>
-      </c>
-      <c r="I49" s="2">
-        <f t="shared" si="5"/>
-        <v>1.9945000000003432E-3</v>
-      </c>
-    </row>
-    <row r="50" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
-        <v>50</v>
-      </c>
-      <c r="D50">
-        <v>20.354033999999999</v>
-      </c>
-      <c r="E50" s="2">
-        <f t="shared" si="4"/>
-        <v>3.9647999999985473E-3</v>
-      </c>
-      <c r="G50" t="s">
-        <v>50</v>
-      </c>
-      <c r="H50">
-        <v>13.266348499999999</v>
-      </c>
-      <c r="I50" s="2">
-        <f t="shared" si="5"/>
-        <v>2.9669999999999419E-3</v>
-      </c>
-    </row>
-    <row r="51" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
         <v>51</v>
       </c>
@@ -2159,7 +2642,7 @@
         <v>20.3560287</v>
       </c>
       <c r="E51" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.9947000000009041E-3</v>
       </c>
       <c r="G51" t="s">
@@ -2169,11 +2652,31 @@
         <v>13.268343399999999</v>
       </c>
       <c r="I51" s="2">
+        <f t="shared" si="7"/>
+        <v>1.9948999999996886E-3</v>
+      </c>
+      <c r="K51" t="s">
+        <v>51</v>
+      </c>
+      <c r="L51">
+        <v>13.342173600000001</v>
+      </c>
+      <c r="M51" s="2">
+        <f t="shared" si="4"/>
+        <v>1.9930999999999699E-3</v>
+      </c>
+      <c r="O51" t="s">
+        <v>51</v>
+      </c>
+      <c r="P51">
+        <v>13.501185899999999</v>
+      </c>
+      <c r="Q51" s="2">
         <f t="shared" si="5"/>
-        <v>1.9948999999996886E-3</v>
-      </c>
-    </row>
-    <row r="52" spans="3:9" x14ac:dyDescent="0.25">
+        <v>2.9904999999992299E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>52</v>
       </c>
@@ -2181,7 +2684,7 @@
         <v>20.359049899999999</v>
       </c>
       <c r="E52" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.021199999999169E-3</v>
       </c>
       <c r="G52" t="s">
@@ -2191,11 +2694,31 @@
         <v>13.271335300000001</v>
       </c>
       <c r="I52" s="2">
+        <f t="shared" si="7"/>
+        <v>2.9919000000013796E-3</v>
+      </c>
+      <c r="K52" t="s">
+        <v>52</v>
+      </c>
+      <c r="L52">
+        <v>13.344169000000001</v>
+      </c>
+      <c r="M52" s="2">
+        <f t="shared" si="4"/>
+        <v>1.9954000000002026E-3</v>
+      </c>
+      <c r="O52" t="s">
+        <v>52</v>
+      </c>
+      <c r="P52">
+        <v>13.503228500000001</v>
+      </c>
+      <c r="Q52" s="2">
         <f t="shared" si="5"/>
-        <v>2.9919000000013796E-3</v>
-      </c>
-    </row>
-    <row r="53" spans="3:9" x14ac:dyDescent="0.25">
+        <v>2.0426000000011157E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
         <v>53</v>
       </c>
@@ -2203,7 +2726,7 @@
         <v>20.361014900000001</v>
       </c>
       <c r="E53" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.9650000000019929E-3</v>
       </c>
       <c r="G53" t="s">
@@ -2213,11 +2736,31 @@
         <v>13.274327299999999</v>
       </c>
       <c r="I53" s="2">
+        <f t="shared" si="7"/>
+        <v>2.9919999999989955E-3</v>
+      </c>
+      <c r="K53" t="s">
+        <v>53</v>
+      </c>
+      <c r="L53">
+        <v>13.347161</v>
+      </c>
+      <c r="M53" s="2">
+        <f t="shared" si="4"/>
+        <v>2.9919999999989955E-3</v>
+      </c>
+      <c r="O53" t="s">
+        <v>53</v>
+      </c>
+      <c r="P53">
+        <v>13.506147800000001</v>
+      </c>
+      <c r="Q53" s="2">
         <f t="shared" si="5"/>
-        <v>2.9919999999989955E-3</v>
-      </c>
-    </row>
-    <row r="54" spans="3:9" x14ac:dyDescent="0.25">
+        <v>2.9193000000002911E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
         <v>54</v>
       </c>
@@ -2225,7 +2768,7 @@
         <v>20.3630347</v>
       </c>
       <c r="E54" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.0197999999993499E-3</v>
       </c>
       <c r="G54" t="s">
@@ -2235,11 +2778,31 @@
         <v>13.2763223</v>
       </c>
       <c r="I54" s="2">
+        <f t="shared" si="7"/>
+        <v>1.9950000000008572E-3</v>
+      </c>
+      <c r="K54" t="s">
+        <v>54</v>
+      </c>
+      <c r="L54">
+        <v>13.349155</v>
+      </c>
+      <c r="M54" s="2">
+        <f t="shared" si="4"/>
+        <v>1.9939999999998292E-3</v>
+      </c>
+      <c r="O54" t="s">
+        <v>54</v>
+      </c>
+      <c r="P54">
+        <v>13.508142400000001</v>
+      </c>
+      <c r="Q54" s="2">
         <f t="shared" si="5"/>
-        <v>1.9950000000008572E-3</v>
-      </c>
-    </row>
-    <row r="55" spans="3:9" x14ac:dyDescent="0.25">
+        <v>1.9945999999997355E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
         <v>55</v>
       </c>
@@ -2247,7 +2810,7 @@
         <v>20.3660274</v>
       </c>
       <c r="E55" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.9927000000000703E-3</v>
       </c>
       <c r="G55" t="s">
@@ -2257,11 +2820,31 @@
         <v>13.280336399999999</v>
       </c>
       <c r="I55" s="2">
+        <f t="shared" si="7"/>
+        <v>4.0140999999991323E-3</v>
+      </c>
+      <c r="K55" t="s">
+        <v>55</v>
+      </c>
+      <c r="L55">
+        <v>13.3511498</v>
+      </c>
+      <c r="M55" s="2">
+        <f t="shared" si="4"/>
+        <v>1.9948000000002963E-3</v>
+      </c>
+      <c r="O55" t="s">
+        <v>55</v>
+      </c>
+      <c r="P55">
+        <v>13.5131546</v>
+      </c>
+      <c r="Q55" s="2">
         <f t="shared" si="5"/>
-        <v>4.0140999999991323E-3</v>
-      </c>
-    </row>
-    <row r="56" spans="3:9" x14ac:dyDescent="0.25">
+        <v>5.0121999999994671E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
         <v>56</v>
       </c>
@@ -2269,7 +2852,7 @@
         <v>20.367996099999999</v>
       </c>
       <c r="E56" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.9686999999990462E-3</v>
       </c>
       <c r="G56" t="s">
@@ -2279,11 +2862,31 @@
         <v>13.2823063</v>
       </c>
       <c r="I56" s="2">
+        <f t="shared" si="7"/>
+        <v>1.969900000000635E-3</v>
+      </c>
+      <c r="K56" t="s">
+        <v>56</v>
+      </c>
+      <c r="L56">
+        <v>13.3541416</v>
+      </c>
+      <c r="M56" s="2">
+        <f t="shared" si="4"/>
+        <v>2.991800000000211E-3</v>
+      </c>
+      <c r="O56" t="s">
+        <v>56</v>
+      </c>
+      <c r="P56">
+        <v>13.5151485</v>
+      </c>
+      <c r="Q56" s="2">
         <f t="shared" si="5"/>
-        <v>1.969900000000635E-3</v>
-      </c>
-    </row>
-    <row r="57" spans="3:9" x14ac:dyDescent="0.25">
+        <v>1.993900000000437E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
         <v>57</v>
       </c>
@@ -2291,7 +2894,7 @@
         <v>20.370989099999999</v>
       </c>
       <c r="E57" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.9930000000000234E-3</v>
       </c>
       <c r="G57" t="s">
@@ -2301,11 +2904,31 @@
         <v>13.285298600000001</v>
       </c>
       <c r="I57" s="2">
+        <f t="shared" si="7"/>
+        <v>2.9923000000007249E-3</v>
+      </c>
+      <c r="K57" t="s">
+        <v>57</v>
+      </c>
+      <c r="L57">
+        <v>13.3561362</v>
+      </c>
+      <c r="M57" s="2">
+        <f t="shared" si="4"/>
+        <v>1.9945999999997355E-3</v>
+      </c>
+      <c r="O57" t="s">
+        <v>57</v>
+      </c>
+      <c r="P57">
+        <v>13.518140300000001</v>
+      </c>
+      <c r="Q57" s="2">
         <f t="shared" si="5"/>
-        <v>2.9923000000007249E-3</v>
-      </c>
-    </row>
-    <row r="58" spans="3:9" x14ac:dyDescent="0.25">
+        <v>2.991800000000211E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
         <v>32</v>
       </c>
@@ -2313,7 +2936,7 @@
         <v>31.068190999999999</v>
       </c>
       <c r="E58" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10.6972019</v>
       </c>
       <c r="G58" t="s">
@@ -2323,11 +2946,31 @@
         <v>19.540128299999999</v>
       </c>
       <c r="I58" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6.2548296999999984</v>
       </c>
-    </row>
-    <row r="59" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K58" t="s">
+        <v>32</v>
+      </c>
+      <c r="L58">
+        <v>16.918050900000001</v>
+      </c>
+      <c r="M58" s="2">
+        <f t="shared" ref="M58:M109" si="8">L58-L57</f>
+        <v>3.5619147000000009</v>
+      </c>
+      <c r="O58" t="s">
+        <v>32</v>
+      </c>
+      <c r="P58">
+        <v>16.641889599999999</v>
+      </c>
+      <c r="Q58" s="2">
+        <f t="shared" ref="Q58:Q109" si="9">P58-P57</f>
+        <v>3.1237492999999983</v>
+      </c>
+    </row>
+    <row r="59" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>33</v>
       </c>
@@ -2335,7 +2978,7 @@
         <v>42.085525099999998</v>
       </c>
       <c r="E59" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>11.017334099999999</v>
       </c>
       <c r="G59" t="s">
@@ -2345,11 +2988,31 @@
         <v>25.648947799999998</v>
       </c>
       <c r="I59" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6.1088194999999992</v>
       </c>
-    </row>
-    <row r="60" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K59" t="s">
+        <v>33</v>
+      </c>
+      <c r="L59">
+        <v>20.413237899999999</v>
+      </c>
+      <c r="M59" s="2">
+        <f t="shared" si="8"/>
+        <v>3.4951869999999978</v>
+      </c>
+      <c r="O59" t="s">
+        <v>33</v>
+      </c>
+      <c r="P59">
+        <v>19.635462700000001</v>
+      </c>
+      <c r="Q59" s="2">
+        <f t="shared" si="9"/>
+        <v>2.9935731000000025</v>
+      </c>
+    </row>
+    <row r="60" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
         <v>34</v>
       </c>
@@ -2357,7 +3020,7 @@
         <v>54.290973800000003</v>
       </c>
       <c r="E60" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>12.205448700000005</v>
       </c>
       <c r="G60" t="s">
@@ -2367,11 +3030,31 @@
         <v>31.802139400000002</v>
       </c>
       <c r="I60" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6.1531916000000031</v>
       </c>
-    </row>
-    <row r="61" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K60" t="s">
+        <v>34</v>
+      </c>
+      <c r="L60">
+        <v>23.956774500000002</v>
+      </c>
+      <c r="M60" s="2">
+        <f t="shared" si="8"/>
+        <v>3.543536600000003</v>
+      </c>
+      <c r="O60" t="s">
+        <v>34</v>
+      </c>
+      <c r="P60">
+        <v>23.989902000000001</v>
+      </c>
+      <c r="Q60" s="2">
+        <f t="shared" si="9"/>
+        <v>4.3544392999999992</v>
+      </c>
+    </row>
+    <row r="61" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
         <v>35</v>
       </c>
@@ -2379,7 +3062,7 @@
         <v>65.753210199999998</v>
       </c>
       <c r="E61" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>11.462236399999995</v>
       </c>
       <c r="G61" t="s">
@@ -2389,11 +3072,31 @@
         <v>38.012390699999997</v>
       </c>
       <c r="I61" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6.2102512999999959</v>
       </c>
-    </row>
-    <row r="62" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K61" t="s">
+        <v>35</v>
+      </c>
+      <c r="L61">
+        <v>27.449572100000001</v>
+      </c>
+      <c r="M61" s="2">
+        <f t="shared" si="8"/>
+        <v>3.4927975999999994</v>
+      </c>
+      <c r="O61" t="s">
+        <v>35</v>
+      </c>
+      <c r="P61">
+        <v>28.361383100000001</v>
+      </c>
+      <c r="Q61" s="2">
+        <f t="shared" si="9"/>
+        <v>4.3714811000000005</v>
+      </c>
+    </row>
+    <row r="62" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
         <v>58</v>
       </c>
@@ -2401,7 +3104,7 @@
         <v>76.701430000000002</v>
       </c>
       <c r="E62" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10.948219800000004</v>
       </c>
       <c r="G62" t="s">
@@ -2411,11 +3114,31 @@
         <v>44.217797500000003</v>
       </c>
       <c r="I62" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6.2054068000000058</v>
       </c>
-    </row>
-    <row r="63" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K62" t="s">
+        <v>58</v>
+      </c>
+      <c r="L62">
+        <v>30.9678094</v>
+      </c>
+      <c r="M62" s="2">
+        <f t="shared" si="8"/>
+        <v>3.5182372999999991</v>
+      </c>
+      <c r="O62" t="s">
+        <v>58</v>
+      </c>
+      <c r="P62">
+        <v>33.0408799</v>
+      </c>
+      <c r="Q62" s="2">
+        <f t="shared" si="9"/>
+        <v>4.679496799999999</v>
+      </c>
+    </row>
+    <row r="63" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
         <v>59</v>
       </c>
@@ -2423,7 +3146,7 @@
         <v>87.925368199999994</v>
       </c>
       <c r="E63" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>11.223938199999992</v>
       </c>
       <c r="G63" t="s">
@@ -2433,11 +3156,31 @@
         <v>51.330630499999998</v>
       </c>
       <c r="I63" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7.1128329999999949</v>
       </c>
-    </row>
-    <row r="64" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K63" t="s">
+        <v>59</v>
+      </c>
+      <c r="L63">
+        <v>35.143852299999999</v>
+      </c>
+      <c r="M63" s="2">
+        <f t="shared" si="8"/>
+        <v>4.1760428999999988</v>
+      </c>
+      <c r="O63" t="s">
+        <v>59</v>
+      </c>
+      <c r="P63">
+        <v>38.582099700000001</v>
+      </c>
+      <c r="Q63" s="2">
+        <f t="shared" si="9"/>
+        <v>5.5412198000000004</v>
+      </c>
+    </row>
+    <row r="64" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
         <v>60</v>
       </c>
@@ -2445,7 +3188,7 @@
         <v>97.905528099999998</v>
       </c>
       <c r="E64" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.9801599000000039</v>
       </c>
       <c r="G64" t="s">
@@ -2455,11 +3198,31 @@
         <v>58.764271200000003</v>
       </c>
       <c r="I64" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7.4336407000000051</v>
       </c>
-    </row>
-    <row r="65" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K64" t="s">
+        <v>60</v>
+      </c>
+      <c r="L64">
+        <v>39.291057700000003</v>
+      </c>
+      <c r="M64" s="2">
+        <f t="shared" si="8"/>
+        <v>4.1472054000000043</v>
+      </c>
+      <c r="O64" t="s">
+        <v>60</v>
+      </c>
+      <c r="P64">
+        <v>43.507315400000003</v>
+      </c>
+      <c r="Q64" s="2">
+        <f t="shared" si="9"/>
+        <v>4.9252157000000025</v>
+      </c>
+    </row>
+    <row r="65" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
         <v>61</v>
       </c>
@@ -2467,7 +3230,7 @@
         <v>108.046451</v>
       </c>
       <c r="E65" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10.140922900000007</v>
       </c>
       <c r="G65" t="s">
@@ -2477,11 +3240,31 @@
         <v>65.835171700000004</v>
       </c>
       <c r="I65" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7.0709005000000005</v>
       </c>
-    </row>
-    <row r="66" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K65" t="s">
+        <v>61</v>
+      </c>
+      <c r="L65">
+        <v>43.4754632</v>
+      </c>
+      <c r="M65" s="2">
+        <f t="shared" si="8"/>
+        <v>4.1844054999999969</v>
+      </c>
+      <c r="O65" t="s">
+        <v>61</v>
+      </c>
+      <c r="P65">
+        <v>48.094173599999998</v>
+      </c>
+      <c r="Q65" s="2">
+        <f t="shared" si="9"/>
+        <v>4.5868581999999947</v>
+      </c>
+    </row>
+    <row r="66" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
         <v>62</v>
       </c>
@@ -2489,7 +3272,7 @@
         <v>118.2703604</v>
       </c>
       <c r="E66" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10.223909399999997</v>
       </c>
       <c r="G66" t="s">
@@ -2499,11 +3282,31 @@
         <v>72.871932099999995</v>
       </c>
       <c r="I66" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7.0367603999999915</v>
       </c>
-    </row>
-    <row r="67" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K66" t="s">
+        <v>62</v>
+      </c>
+      <c r="L66">
+        <v>47.658663699999998</v>
+      </c>
+      <c r="M66" s="2">
+        <f t="shared" si="8"/>
+        <v>4.1832004999999981</v>
+      </c>
+      <c r="O66" t="s">
+        <v>62</v>
+      </c>
+      <c r="P66">
+        <v>52.593810499999996</v>
+      </c>
+      <c r="Q66" s="2">
+        <f t="shared" si="9"/>
+        <v>4.4996368999999987</v>
+      </c>
+    </row>
+    <row r="67" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
         <v>63</v>
       </c>
@@ -2511,7 +3314,7 @@
         <v>129.3465521</v>
       </c>
       <c r="E67" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>11.076191699999995</v>
       </c>
       <c r="G67" t="s">
@@ -2521,11 +3324,31 @@
         <v>80.045381399999997</v>
       </c>
       <c r="I67" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7.1734493000000015</v>
       </c>
-    </row>
-    <row r="68" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K67" t="s">
+        <v>63</v>
+      </c>
+      <c r="L67">
+        <v>51.859041599999998</v>
+      </c>
+      <c r="M67" s="2">
+        <f t="shared" si="8"/>
+        <v>4.2003778999999994</v>
+      </c>
+      <c r="O67" t="s">
+        <v>63</v>
+      </c>
+      <c r="P67">
+        <v>56.040461200000003</v>
+      </c>
+      <c r="Q67" s="2">
+        <f t="shared" si="9"/>
+        <v>3.4466507000000064</v>
+      </c>
+    </row>
+    <row r="68" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
         <v>64</v>
       </c>
@@ -2533,7 +3356,7 @@
         <v>141.16064549999999</v>
       </c>
       <c r="E68" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>11.81409339999999</v>
       </c>
       <c r="G68" t="s">
@@ -2543,11 +3366,31 @@
         <v>87.297029699999996</v>
       </c>
       <c r="I68" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7.2516482999999994</v>
       </c>
-    </row>
-    <row r="69" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K68" t="s">
+        <v>64</v>
+      </c>
+      <c r="L68">
+        <v>56.071149499999997</v>
+      </c>
+      <c r="M68" s="2">
+        <f t="shared" si="8"/>
+        <v>4.2121078999999995</v>
+      </c>
+      <c r="O68" t="s">
+        <v>64</v>
+      </c>
+      <c r="P68">
+        <v>59.691591099999997</v>
+      </c>
+      <c r="Q68" s="2">
+        <f t="shared" si="9"/>
+        <v>3.6511298999999937</v>
+      </c>
+    </row>
+    <row r="69" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
         <v>65</v>
       </c>
@@ -2555,7 +3398,7 @@
         <v>152.28584739999999</v>
       </c>
       <c r="E69" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>11.125201900000008</v>
       </c>
       <c r="G69" t="s">
@@ -2565,11 +3408,31 @@
         <v>95.166673000000003</v>
       </c>
       <c r="I69" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7.869643300000007</v>
       </c>
-    </row>
-    <row r="70" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K69" t="s">
+        <v>65</v>
+      </c>
+      <c r="L69">
+        <v>60.430204199999999</v>
+      </c>
+      <c r="M69" s="2">
+        <f t="shared" si="8"/>
+        <v>4.3590547000000015</v>
+      </c>
+      <c r="O69" t="s">
+        <v>65</v>
+      </c>
+      <c r="P69">
+        <v>63.215424300000002</v>
+      </c>
+      <c r="Q69" s="2">
+        <f t="shared" si="9"/>
+        <v>3.5238332000000057</v>
+      </c>
+    </row>
+    <row r="70" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
         <v>66</v>
       </c>
@@ -2577,7 +3440,7 @@
         <v>160.95311899999999</v>
       </c>
       <c r="E70" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8.6672715999999923</v>
       </c>
       <c r="G70" t="s">
@@ -2587,11 +3450,31 @@
         <v>103.0454464</v>
       </c>
       <c r="I70" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7.8787734</v>
       </c>
-    </row>
-    <row r="71" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K70" t="s">
+        <v>66</v>
+      </c>
+      <c r="L70">
+        <v>64.8545357</v>
+      </c>
+      <c r="M70" s="2">
+        <f t="shared" si="8"/>
+        <v>4.424331500000001</v>
+      </c>
+      <c r="O70" t="s">
+        <v>66</v>
+      </c>
+      <c r="P70">
+        <v>66.782382799999993</v>
+      </c>
+      <c r="Q70" s="2">
+        <f t="shared" si="9"/>
+        <v>3.5669584999999913</v>
+      </c>
+    </row>
+    <row r="71" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
         <v>67</v>
       </c>
@@ -2599,7 +3482,7 @@
         <v>169.7560484</v>
       </c>
       <c r="E71" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8.8029294000000107</v>
       </c>
       <c r="G71" t="s">
@@ -2609,11 +3492,31 @@
         <v>111.0662859</v>
       </c>
       <c r="I71" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8.0208394999999939</v>
       </c>
-    </row>
-    <row r="72" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K71" t="s">
+        <v>67</v>
+      </c>
+      <c r="L71">
+        <v>69.2502815</v>
+      </c>
+      <c r="M71" s="2">
+        <f t="shared" si="8"/>
+        <v>4.3957458000000003</v>
+      </c>
+      <c r="O71" t="s">
+        <v>67</v>
+      </c>
+      <c r="P71">
+        <v>70.414761100000007</v>
+      </c>
+      <c r="Q71" s="2">
+        <f t="shared" si="9"/>
+        <v>3.6323783000000134</v>
+      </c>
+    </row>
+    <row r="72" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
         <v>68</v>
       </c>
@@ -2621,7 +3524,7 @@
         <v>178.6769137</v>
       </c>
       <c r="E72" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8.9208653000000027</v>
       </c>
       <c r="G72" t="s">
@@ -2631,11 +3534,31 @@
         <v>119.1812479</v>
       </c>
       <c r="I72" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8.1149620000000056</v>
       </c>
-    </row>
-    <row r="73" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K72" t="s">
+        <v>68</v>
+      </c>
+      <c r="L72">
+        <v>73.684854700000002</v>
+      </c>
+      <c r="M72" s="2">
+        <f t="shared" si="8"/>
+        <v>4.4345732000000027</v>
+      </c>
+      <c r="O72" t="s">
+        <v>68</v>
+      </c>
+      <c r="P72">
+        <v>74.642528299999995</v>
+      </c>
+      <c r="Q72" s="2">
+        <f t="shared" si="9"/>
+        <v>4.2277671999999882</v>
+      </c>
+    </row>
+    <row r="73" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
         <v>69</v>
       </c>
@@ -2643,7 +3566,7 @@
         <v>187.2575559</v>
       </c>
       <c r="E73" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8.5806421999999998</v>
       </c>
       <c r="G73" t="s">
@@ -2653,11 +3576,31 @@
         <v>127.16368559999999</v>
       </c>
       <c r="I73" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7.9824376999999913</v>
       </c>
-    </row>
-    <row r="74" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K73" t="s">
+        <v>69</v>
+      </c>
+      <c r="L73">
+        <v>78.154358900000005</v>
+      </c>
+      <c r="M73" s="2">
+        <f t="shared" si="8"/>
+        <v>4.4695042000000029</v>
+      </c>
+      <c r="O73" t="s">
+        <v>69</v>
+      </c>
+      <c r="P73">
+        <v>78.765921199999994</v>
+      </c>
+      <c r="Q73" s="2">
+        <f t="shared" si="9"/>
+        <v>4.1233928999999989</v>
+      </c>
+    </row>
+    <row r="74" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
         <v>70</v>
       </c>
@@ -2665,7 +3608,7 @@
         <v>196.01606269999999</v>
       </c>
       <c r="E74" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8.7585067999999922</v>
       </c>
       <c r="G74" t="s">
@@ -2675,11 +3618,31 @@
         <v>135.50220049999999</v>
       </c>
       <c r="I74" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8.3385148999999927</v>
       </c>
-    </row>
-    <row r="75" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K74" t="s">
+        <v>70</v>
+      </c>
+      <c r="L74">
+        <v>82.618960200000004</v>
+      </c>
+      <c r="M74" s="2">
+        <f t="shared" si="8"/>
+        <v>4.4646012999999982</v>
+      </c>
+      <c r="O74" t="s">
+        <v>70</v>
+      </c>
+      <c r="P74">
+        <v>82.980727299999998</v>
+      </c>
+      <c r="Q74" s="2">
+        <f t="shared" si="9"/>
+        <v>4.2148061000000041</v>
+      </c>
+    </row>
+    <row r="75" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
         <v>71</v>
       </c>
@@ -2687,7 +3650,7 @@
         <v>203.94664739999999</v>
       </c>
       <c r="E75" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7.9305846999999972</v>
       </c>
       <c r="G75" t="s">
@@ -2697,11 +3660,31 @@
         <v>143.43515289999999</v>
       </c>
       <c r="I75" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7.9329524000000049</v>
       </c>
-    </row>
-    <row r="76" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K75" t="s">
+        <v>71</v>
+      </c>
+      <c r="L75">
+        <v>87.335482299999995</v>
+      </c>
+      <c r="M75" s="2">
+        <f t="shared" si="8"/>
+        <v>4.7165220999999917</v>
+      </c>
+      <c r="O75" t="s">
+        <v>71</v>
+      </c>
+      <c r="P75">
+        <v>87.224450599999997</v>
+      </c>
+      <c r="Q75" s="2">
+        <f t="shared" si="9"/>
+        <v>4.2437232999999992</v>
+      </c>
+    </row>
+    <row r="76" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
         <v>72</v>
       </c>
@@ -2709,7 +3692,7 @@
         <v>213.1985238</v>
       </c>
       <c r="E76" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.2518764000000147</v>
       </c>
       <c r="G76" t="s">
@@ -2719,11 +3702,31 @@
         <v>151.69467789999999</v>
       </c>
       <c r="I76" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8.2595249999999965</v>
       </c>
-    </row>
-    <row r="77" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K76" t="s">
+        <v>72</v>
+      </c>
+      <c r="L76">
+        <v>90.563846999999996</v>
+      </c>
+      <c r="M76" s="2">
+        <f t="shared" si="8"/>
+        <v>3.2283647000000002</v>
+      </c>
+      <c r="O76" t="s">
+        <v>72</v>
+      </c>
+      <c r="P76">
+        <v>91.463509700000003</v>
+      </c>
+      <c r="Q76" s="2">
+        <f t="shared" si="9"/>
+        <v>4.2390591000000057</v>
+      </c>
+    </row>
+    <row r="77" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
         <v>73</v>
       </c>
@@ -2731,7 +3734,7 @@
         <v>221.6058007</v>
       </c>
       <c r="E77" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8.4072768999999994</v>
       </c>
       <c r="G77" t="s">
@@ -2741,11 +3744,31 @@
         <v>162.73395970000001</v>
       </c>
       <c r="I77" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>11.039281800000026</v>
       </c>
-    </row>
-    <row r="78" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K77" t="s">
+        <v>73</v>
+      </c>
+      <c r="L77">
+        <v>93.829155999999998</v>
+      </c>
+      <c r="M77" s="2">
+        <f t="shared" si="8"/>
+        <v>3.265309000000002</v>
+      </c>
+      <c r="O77" t="s">
+        <v>73</v>
+      </c>
+      <c r="P77">
+        <v>95.879664700000006</v>
+      </c>
+      <c r="Q77" s="2">
+        <f t="shared" si="9"/>
+        <v>4.4161550000000034</v>
+      </c>
+    </row>
+    <row r="78" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
         <v>74</v>
       </c>
@@ -2753,7 +3776,7 @@
         <v>230.0946654</v>
       </c>
       <c r="E78" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8.4888646999999935</v>
       </c>
       <c r="G78" t="s">
@@ -2763,11 +3786,31 @@
         <v>170.83209239999999</v>
       </c>
       <c r="I78" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8.0981326999999794</v>
       </c>
-    </row>
-    <row r="79" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K78" t="s">
+        <v>74</v>
+      </c>
+      <c r="L78">
+        <v>97.092476899999994</v>
+      </c>
+      <c r="M78" s="2">
+        <f t="shared" si="8"/>
+        <v>3.2633208999999965</v>
+      </c>
+      <c r="O78" t="s">
+        <v>74</v>
+      </c>
+      <c r="P78">
+        <v>101.43481559999999</v>
+      </c>
+      <c r="Q78" s="2">
+        <f t="shared" si="9"/>
+        <v>5.5551508999999868</v>
+      </c>
+    </row>
+    <row r="79" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
         <v>75</v>
       </c>
@@ -2775,7 +3818,7 @@
         <v>238.544726</v>
       </c>
       <c r="E79" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8.4500606000000005</v>
       </c>
       <c r="G79" t="s">
@@ -2785,11 +3828,31 @@
         <v>178.99932129999999</v>
       </c>
       <c r="I79" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8.1672288999999978</v>
       </c>
-    </row>
-    <row r="80" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K79" t="s">
+        <v>75</v>
+      </c>
+      <c r="L79">
+        <v>100.3457599</v>
+      </c>
+      <c r="M79" s="2">
+        <f t="shared" si="8"/>
+        <v>3.2532830000000104</v>
+      </c>
+      <c r="O79" t="s">
+        <v>75</v>
+      </c>
+      <c r="P79">
+        <v>106.82638969999999</v>
+      </c>
+      <c r="Q79" s="2">
+        <f t="shared" si="9"/>
+        <v>5.3915740999999997</v>
+      </c>
+    </row>
+    <row r="80" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
         <v>76</v>
       </c>
@@ -2797,7 +3860,7 @@
         <v>247.12502330000001</v>
       </c>
       <c r="E80" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8.5802973000000122</v>
       </c>
       <c r="G80" t="s">
@@ -2807,11 +3870,31 @@
         <v>187.29363079999999</v>
       </c>
       <c r="I80" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8.2943094999999971</v>
       </c>
-    </row>
-    <row r="81" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K80" t="s">
+        <v>76</v>
+      </c>
+      <c r="L80">
+        <v>103.5964719</v>
+      </c>
+      <c r="M80" s="2">
+        <f t="shared" si="8"/>
+        <v>3.2507119999999929</v>
+      </c>
+      <c r="O80" t="s">
+        <v>76</v>
+      </c>
+      <c r="P80">
+        <v>112.1115696</v>
+      </c>
+      <c r="Q80" s="2">
+        <f t="shared" si="9"/>
+        <v>5.2851799000000028</v>
+      </c>
+    </row>
+    <row r="81" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
         <v>77</v>
       </c>
@@ -2819,7 +3902,7 @@
         <v>255.0500328</v>
       </c>
       <c r="E81" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7.9250094999999874</v>
       </c>
       <c r="G81" t="s">
@@ -2829,11 +3912,31 @@
         <v>196.76437300000001</v>
       </c>
       <c r="I81" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9.4707422000000179</v>
       </c>
-    </row>
-    <row r="82" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K81" t="s">
+        <v>77</v>
+      </c>
+      <c r="L81">
+        <v>106.90482</v>
+      </c>
+      <c r="M81" s="2">
+        <f t="shared" si="8"/>
+        <v>3.3083481000000035</v>
+      </c>
+      <c r="O81" t="s">
+        <v>77</v>
+      </c>
+      <c r="P81">
+        <v>117.42045539999999</v>
+      </c>
+      <c r="Q81" s="2">
+        <f t="shared" si="9"/>
+        <v>5.3088857999999988</v>
+      </c>
+    </row>
+    <row r="82" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
         <v>78</v>
       </c>
@@ -2841,7 +3944,7 @@
         <v>266.33621040000003</v>
       </c>
       <c r="E82" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>11.28617760000003</v>
       </c>
       <c r="G82" t="s">
@@ -2851,11 +3954,31 @@
         <v>206.41274189999999</v>
       </c>
       <c r="I82" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9.6483688999999799</v>
       </c>
-    </row>
-    <row r="83" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K82" t="s">
+        <v>78</v>
+      </c>
+      <c r="L82">
+        <v>110.1919039</v>
+      </c>
+      <c r="M82" s="2">
+        <f t="shared" si="8"/>
+        <v>3.2870838999999989</v>
+      </c>
+      <c r="O82" t="s">
+        <v>78</v>
+      </c>
+      <c r="P82">
+        <v>122.5054931</v>
+      </c>
+      <c r="Q82" s="2">
+        <f t="shared" si="9"/>
+        <v>5.0850377000000009</v>
+      </c>
+    </row>
+    <row r="83" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C83" t="s">
         <v>36</v>
       </c>
@@ -2863,7 +3986,7 @@
         <v>279.21048560000003</v>
       </c>
       <c r="E83" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>12.8742752</v>
       </c>
       <c r="G83" t="s">
@@ -2873,11 +3996,31 @@
         <v>217.13535880000001</v>
       </c>
       <c r="I83" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>10.72261690000002</v>
       </c>
-    </row>
-    <row r="84" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K83" t="s">
+        <v>36</v>
+      </c>
+      <c r="L83">
+        <v>119.82257079999999</v>
+      </c>
+      <c r="M83" s="2">
+        <f t="shared" si="8"/>
+        <v>9.6306668999999943</v>
+      </c>
+      <c r="O83" t="s">
+        <v>36</v>
+      </c>
+      <c r="P83">
+        <v>131.8394629</v>
+      </c>
+      <c r="Q83" s="2">
+        <f t="shared" si="9"/>
+        <v>9.3339698000000055</v>
+      </c>
+    </row>
+    <row r="84" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
         <v>15</v>
       </c>
@@ -2885,7 +4028,7 @@
         <v>283.60751370000003</v>
       </c>
       <c r="E84" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.3970281</v>
       </c>
       <c r="G84" t="s">
@@ -2895,11 +4038,31 @@
         <v>220.0280813</v>
       </c>
       <c r="I84" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.8927224999999908</v>
       </c>
-    </row>
-    <row r="85" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K84" t="s">
+        <v>15</v>
+      </c>
+      <c r="L84">
+        <v>122.19943840000001</v>
+      </c>
+      <c r="M84" s="2">
+        <f t="shared" si="8"/>
+        <v>2.3768676000000113</v>
+      </c>
+      <c r="O84" t="s">
+        <v>15</v>
+      </c>
+      <c r="P84">
+        <v>134.50635650000001</v>
+      </c>
+      <c r="Q84" s="2">
+        <f t="shared" si="9"/>
+        <v>2.6668936000000087</v>
+      </c>
+    </row>
+    <row r="85" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C85" t="s">
         <v>16</v>
       </c>
@@ -2907,7 +4070,7 @@
         <v>287.70795930000003</v>
       </c>
       <c r="E85" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.1004456000000005</v>
       </c>
       <c r="G85" t="s">
@@ -2917,11 +4080,31 @@
         <v>222.88774280000001</v>
       </c>
       <c r="I85" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.8596615000000156</v>
       </c>
-    </row>
-    <row r="86" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K85" t="s">
+        <v>16</v>
+      </c>
+      <c r="L85">
+        <v>124.4862679</v>
+      </c>
+      <c r="M85" s="2">
+        <f t="shared" si="8"/>
+        <v>2.2868294999999961</v>
+      </c>
+      <c r="O85" t="s">
+        <v>16</v>
+      </c>
+      <c r="P85">
+        <v>136.96378340000001</v>
+      </c>
+      <c r="Q85" s="2">
+        <f t="shared" si="9"/>
+        <v>2.4574269000000015</v>
+      </c>
+    </row>
+    <row r="86" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C86" t="s">
         <v>17</v>
       </c>
@@ -2929,7 +4112,7 @@
         <v>291.82098079999997</v>
       </c>
       <c r="E86" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.1130214999999453</v>
       </c>
       <c r="G86" t="s">
@@ -2939,11 +4122,31 @@
         <v>225.8321795</v>
       </c>
       <c r="I86" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.9444366999999829</v>
       </c>
-    </row>
-    <row r="87" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K86" t="s">
+        <v>17</v>
+      </c>
+      <c r="L86">
+        <v>126.8149994</v>
+      </c>
+      <c r="M86" s="2">
+        <f t="shared" si="8"/>
+        <v>2.3287315000000035</v>
+      </c>
+      <c r="O86" t="s">
+        <v>17</v>
+      </c>
+      <c r="P86">
+        <v>139.6745425</v>
+      </c>
+      <c r="Q86" s="2">
+        <f t="shared" si="9"/>
+        <v>2.71075909999999</v>
+      </c>
+    </row>
+    <row r="87" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C87" t="s">
         <v>18</v>
       </c>
@@ -2951,7 +4154,7 @@
         <v>295.7487059</v>
       </c>
       <c r="E87" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.9277251000000319</v>
       </c>
       <c r="G87" t="s">
@@ -2961,11 +4164,31 @@
         <v>228.7198022</v>
       </c>
       <c r="I87" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.8876227000000085</v>
       </c>
-    </row>
-    <row r="88" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K87" t="s">
+        <v>18</v>
+      </c>
+      <c r="L87">
+        <v>129.11262450000001</v>
+      </c>
+      <c r="M87" s="2">
+        <f t="shared" si="8"/>
+        <v>2.2976251000000047</v>
+      </c>
+      <c r="O87" t="s">
+        <v>18</v>
+      </c>
+      <c r="P87">
+        <v>142.45023760000001</v>
+      </c>
+      <c r="Q87" s="2">
+        <f t="shared" si="9"/>
+        <v>2.7756951000000072</v>
+      </c>
+    </row>
+    <row r="88" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C88" t="s">
         <v>79</v>
       </c>
@@ -2973,7 +4196,7 @@
         <v>299.70266350000003</v>
       </c>
       <c r="E88" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.9539576000000238</v>
       </c>
       <c r="G88" t="s">
@@ -2983,11 +4206,31 @@
         <v>231.50196800000001</v>
       </c>
       <c r="I88" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.7821658000000014</v>
       </c>
-    </row>
-    <row r="89" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K88" t="s">
+        <v>79</v>
+      </c>
+      <c r="L88">
+        <v>131.41983300000001</v>
+      </c>
+      <c r="M88" s="2">
+        <f t="shared" si="8"/>
+        <v>2.3072085000000015</v>
+      </c>
+      <c r="O88" t="s">
+        <v>79</v>
+      </c>
+      <c r="P88">
+        <v>144.84389680000001</v>
+      </c>
+      <c r="Q88" s="2">
+        <f t="shared" si="9"/>
+        <v>2.3936592000000019</v>
+      </c>
+    </row>
+    <row r="89" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C89" t="s">
         <v>80</v>
       </c>
@@ -2995,7 +4238,7 @@
         <v>303.96507889999998</v>
       </c>
       <c r="E89" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.2624153999999521</v>
       </c>
       <c r="G89" t="s">
@@ -3005,11 +4248,31 @@
         <v>234.32884419999999</v>
       </c>
       <c r="I89" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.8268761999999867</v>
       </c>
-    </row>
-    <row r="90" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K89" t="s">
+        <v>80</v>
+      </c>
+      <c r="L89">
+        <v>133.75836960000001</v>
+      </c>
+      <c r="M89" s="2">
+        <f t="shared" si="8"/>
+        <v>2.3385365999999976</v>
+      </c>
+      <c r="O89" t="s">
+        <v>80</v>
+      </c>
+      <c r="P89">
+        <v>147.28334749999999</v>
+      </c>
+      <c r="Q89" s="2">
+        <f t="shared" si="9"/>
+        <v>2.4394506999999805</v>
+      </c>
+    </row>
+    <row r="90" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C90" t="s">
         <v>81</v>
       </c>
@@ -3017,7 +4280,7 @@
         <v>308.29835320000001</v>
       </c>
       <c r="E90" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.3332743000000278</v>
       </c>
       <c r="G90" t="s">
@@ -3027,11 +4290,31 @@
         <v>237.1490039</v>
       </c>
       <c r="I90" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.8201597000000049</v>
       </c>
-    </row>
-    <row r="91" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K90" t="s">
+        <v>81</v>
+      </c>
+      <c r="L90">
+        <v>136.13970879999999</v>
+      </c>
+      <c r="M90" s="2">
+        <f t="shared" si="8"/>
+        <v>2.3813391999999851</v>
+      </c>
+      <c r="O90" t="s">
+        <v>81</v>
+      </c>
+      <c r="P90">
+        <v>149.85551409999999</v>
+      </c>
+      <c r="Q90" s="2">
+        <f t="shared" si="9"/>
+        <v>2.5721666000000027</v>
+      </c>
+    </row>
+    <row r="91" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C91" t="s">
         <v>82</v>
       </c>
@@ -3039,7 +4322,7 @@
         <v>312.07917450000002</v>
       </c>
       <c r="E91" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.7808213000000137</v>
       </c>
       <c r="G91" t="s">
@@ -3049,11 +4332,31 @@
         <v>240.03471579999999</v>
       </c>
       <c r="I91" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.8857118999999898</v>
       </c>
-    </row>
-    <row r="92" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K91" t="s">
+        <v>82</v>
+      </c>
+      <c r="L91">
+        <v>138.49301579999999</v>
+      </c>
+      <c r="M91" s="2">
+        <f t="shared" si="8"/>
+        <v>2.3533070000000009</v>
+      </c>
+      <c r="O91" t="s">
+        <v>82</v>
+      </c>
+      <c r="P91">
+        <v>152.30030189999999</v>
+      </c>
+      <c r="Q91" s="2">
+        <f t="shared" si="9"/>
+        <v>2.4447878000000003</v>
+      </c>
+    </row>
+    <row r="92" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C92" t="s">
         <v>83</v>
       </c>
@@ -3061,7 +4364,7 @@
         <v>316.01191139999997</v>
       </c>
       <c r="E92" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.9327368999999521</v>
       </c>
       <c r="G92" t="s">
@@ -3071,11 +4374,31 @@
         <v>242.79259429999999</v>
       </c>
       <c r="I92" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.7578785000000039</v>
       </c>
-    </row>
-    <row r="93" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K92" t="s">
+        <v>83</v>
+      </c>
+      <c r="L92">
+        <v>140.86961170000001</v>
+      </c>
+      <c r="M92" s="2">
+        <f t="shared" si="8"/>
+        <v>2.3765959000000123</v>
+      </c>
+      <c r="O92" t="s">
+        <v>83</v>
+      </c>
+      <c r="P92">
+        <v>154.87441849999999</v>
+      </c>
+      <c r="Q92" s="2">
+        <f t="shared" si="9"/>
+        <v>2.5741165999999964</v>
+      </c>
+    </row>
+    <row r="93" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C93" t="s">
         <v>84</v>
       </c>
@@ -3083,7 +4406,7 @@
         <v>320.1283909</v>
       </c>
       <c r="E93" s="2">
-        <f t="shared" ref="E93:E109" si="6">D93-D92</f>
+        <f t="shared" ref="E93:E109" si="10">D93-D92</f>
         <v>4.1164795000000254</v>
       </c>
       <c r="G93" t="s">
@@ -3093,11 +4416,31 @@
         <v>250.30975770000001</v>
       </c>
       <c r="I93" s="2">
-        <f t="shared" ref="I93:I109" si="7">H93-H92</f>
+        <f t="shared" ref="I93:I109" si="11">H93-H92</f>
         <v>7.5171634000000154</v>
       </c>
-    </row>
-    <row r="94" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K93" t="s">
+        <v>84</v>
+      </c>
+      <c r="L93">
+        <v>143.2728462</v>
+      </c>
+      <c r="M93" s="2">
+        <f t="shared" si="8"/>
+        <v>2.4032344999999964</v>
+      </c>
+      <c r="O93" t="s">
+        <v>84</v>
+      </c>
+      <c r="P93">
+        <v>158.34105510000001</v>
+      </c>
+      <c r="Q93" s="2">
+        <f t="shared" si="9"/>
+        <v>3.4666366000000153</v>
+      </c>
+    </row>
+    <row r="94" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C94" t="s">
         <v>85</v>
       </c>
@@ -3105,7 +4448,7 @@
         <v>324.2032969</v>
       </c>
       <c r="E94" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.0749059999999986</v>
       </c>
       <c r="G94" t="s">
@@ -3115,11 +4458,31 @@
         <v>254.1571031</v>
       </c>
       <c r="I94" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3.8473453999999947</v>
       </c>
-    </row>
-    <row r="95" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K94" t="s">
+        <v>85</v>
+      </c>
+      <c r="L94">
+        <v>145.69477459999999</v>
+      </c>
+      <c r="M94" s="2">
+        <f t="shared" si="8"/>
+        <v>2.4219283999999845</v>
+      </c>
+      <c r="O94" t="s">
+        <v>85</v>
+      </c>
+      <c r="P94">
+        <v>161.05797699999999</v>
+      </c>
+      <c r="Q94" s="2">
+        <f t="shared" si="9"/>
+        <v>2.7169218999999885</v>
+      </c>
+    </row>
+    <row r="95" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C95" t="s">
         <v>86</v>
       </c>
@@ -3127,7 +4490,7 @@
         <v>328.16582510000001</v>
       </c>
       <c r="E95" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>3.9625282000000084</v>
       </c>
       <c r="G95" t="s">
@@ -3137,11 +4500,31 @@
         <v>258.00830580000002</v>
       </c>
       <c r="I95" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3.851202700000016</v>
       </c>
-    </row>
-    <row r="96" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K95" t="s">
+        <v>86</v>
+      </c>
+      <c r="L95">
+        <v>148.11398270000001</v>
+      </c>
+      <c r="M95" s="2">
+        <f t="shared" si="8"/>
+        <v>2.4192081000000201</v>
+      </c>
+      <c r="O95" t="s">
+        <v>86</v>
+      </c>
+      <c r="P95">
+        <v>163.71692189999999</v>
+      </c>
+      <c r="Q95" s="2">
+        <f t="shared" si="9"/>
+        <v>2.6589448999999945</v>
+      </c>
+    </row>
+    <row r="96" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C96" t="s">
         <v>87</v>
       </c>
@@ -3149,7 +4532,7 @@
         <v>332.24455230000001</v>
       </c>
       <c r="E96" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.078727200000003</v>
       </c>
       <c r="G96" t="s">
@@ -3159,11 +4542,31 @@
         <v>261.73802610000001</v>
       </c>
       <c r="I96" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3.7297202999999968</v>
       </c>
-    </row>
-    <row r="97" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K96" t="s">
+        <v>87</v>
+      </c>
+      <c r="L96">
+        <v>153.41763270000001</v>
+      </c>
+      <c r="M96" s="2">
+        <f t="shared" si="8"/>
+        <v>5.3036500000000046</v>
+      </c>
+      <c r="O96" t="s">
+        <v>87</v>
+      </c>
+      <c r="P96">
+        <v>166.4309418</v>
+      </c>
+      <c r="Q96" s="2">
+        <f t="shared" si="9"/>
+        <v>2.7140199000000109</v>
+      </c>
+    </row>
+    <row r="97" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C97" t="s">
         <v>88</v>
       </c>
@@ -3171,7 +4574,7 @@
         <v>336.21403729999997</v>
       </c>
       <c r="E97" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>3.9694849999999633</v>
       </c>
       <c r="G97" t="s">
@@ -3181,11 +4584,31 @@
         <v>265.52973470000001</v>
       </c>
       <c r="I97" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3.7917085999999927</v>
       </c>
-    </row>
-    <row r="98" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K97" t="s">
+        <v>88</v>
+      </c>
+      <c r="L97">
+        <v>156.43162240000001</v>
+      </c>
+      <c r="M97" s="2">
+        <f t="shared" si="8"/>
+        <v>3.0139896999999962</v>
+      </c>
+      <c r="O97" t="s">
+        <v>88</v>
+      </c>
+      <c r="P97">
+        <v>169.1158993</v>
+      </c>
+      <c r="Q97" s="2">
+        <f t="shared" si="9"/>
+        <v>2.6849574999999959</v>
+      </c>
+    </row>
+    <row r="98" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C98" t="s">
         <v>89</v>
       </c>
@@ -3193,7 +4616,7 @@
         <v>340.70100789999998</v>
       </c>
       <c r="E98" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.4869706000000065</v>
       </c>
       <c r="G98" t="s">
@@ -3203,11 +4626,31 @@
         <v>269.3177508</v>
       </c>
       <c r="I98" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3.788016099999993</v>
       </c>
-    </row>
-    <row r="99" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K98" t="s">
+        <v>89</v>
+      </c>
+      <c r="L98">
+        <v>159.38956160000001</v>
+      </c>
+      <c r="M98" s="2">
+        <f t="shared" si="8"/>
+        <v>2.9579391999999984</v>
+      </c>
+      <c r="O98" t="s">
+        <v>89</v>
+      </c>
+      <c r="P98">
+        <v>171.69417250000001</v>
+      </c>
+      <c r="Q98" s="2">
+        <f t="shared" si="9"/>
+        <v>2.5782732000000124</v>
+      </c>
+    </row>
+    <row r="99" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C99" t="s">
         <v>90</v>
       </c>
@@ -3215,7 +4658,7 @@
         <v>345.42150789999999</v>
       </c>
       <c r="E99" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.7205000000000155</v>
       </c>
       <c r="G99" t="s">
@@ -3225,11 +4668,31 @@
         <v>273.1314936</v>
       </c>
       <c r="I99" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3.8137428</v>
       </c>
-    </row>
-    <row r="100" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K99" t="s">
+        <v>90</v>
+      </c>
+      <c r="L99">
+        <v>162.2519341</v>
+      </c>
+      <c r="M99" s="2">
+        <f t="shared" si="8"/>
+        <v>2.8623724999999922</v>
+      </c>
+      <c r="O99" t="s">
+        <v>90</v>
+      </c>
+      <c r="P99">
+        <v>174.5206397</v>
+      </c>
+      <c r="Q99" s="2">
+        <f t="shared" si="9"/>
+        <v>2.8264671999999962</v>
+      </c>
+    </row>
+    <row r="100" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C100" t="s">
         <v>91</v>
       </c>
@@ -3237,7 +4700,7 @@
         <v>349.85682489999999</v>
       </c>
       <c r="E100" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.4353169999999977</v>
       </c>
       <c r="G100" t="s">
@@ -3247,11 +4710,31 @@
         <v>276.87838829999998</v>
       </c>
       <c r="I100" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3.7468946999999844</v>
       </c>
-    </row>
-    <row r="101" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K100" t="s">
+        <v>91</v>
+      </c>
+      <c r="L100">
+        <v>165.0021228</v>
+      </c>
+      <c r="M100" s="2">
+        <f t="shared" si="8"/>
+        <v>2.7501886999999954</v>
+      </c>
+      <c r="O100" t="s">
+        <v>91</v>
+      </c>
+      <c r="P100">
+        <v>177.64943210000001</v>
+      </c>
+      <c r="Q100" s="2">
+        <f t="shared" si="9"/>
+        <v>3.1287924000000089</v>
+      </c>
+    </row>
+    <row r="101" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C101" t="s">
         <v>92</v>
       </c>
@@ -3259,7 +4742,7 @@
         <v>354.63219559999999</v>
       </c>
       <c r="E101" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.7753706999999963</v>
       </c>
       <c r="G101" t="s">
@@ -3269,11 +4752,31 @@
         <v>280.25205360000001</v>
       </c>
       <c r="I101" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3.3736653000000274</v>
       </c>
-    </row>
-    <row r="102" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K101" t="s">
+        <v>92</v>
+      </c>
+      <c r="L101">
+        <v>167.6566033</v>
+      </c>
+      <c r="M101" s="2">
+        <f t="shared" si="8"/>
+        <v>2.6544805000000053</v>
+      </c>
+      <c r="O101" t="s">
+        <v>92</v>
+      </c>
+      <c r="P101">
+        <v>180.8219795</v>
+      </c>
+      <c r="Q101" s="2">
+        <f t="shared" si="9"/>
+        <v>3.1725473999999849</v>
+      </c>
+    </row>
+    <row r="102" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C102" t="s">
         <v>93</v>
       </c>
@@ -3281,7 +4784,7 @@
         <v>359.47067320000002</v>
       </c>
       <c r="E102" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.8384776000000329</v>
       </c>
       <c r="G102" t="s">
@@ -3291,11 +4794,31 @@
         <v>283.60504370000001</v>
       </c>
       <c r="I102" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3.3529900999999995</v>
       </c>
-    </row>
-    <row r="103" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K102" t="s">
+        <v>93</v>
+      </c>
+      <c r="L102">
+        <v>170.32321569999999</v>
+      </c>
+      <c r="M102" s="2">
+        <f t="shared" si="8"/>
+        <v>2.6666123999999911</v>
+      </c>
+      <c r="O102" t="s">
+        <v>93</v>
+      </c>
+      <c r="P102">
+        <v>184.09527879999999</v>
+      </c>
+      <c r="Q102" s="2">
+        <f t="shared" si="9"/>
+        <v>3.2732992999999908</v>
+      </c>
+    </row>
+    <row r="103" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C103" t="s">
         <v>94</v>
       </c>
@@ -3303,7 +4826,7 @@
         <v>364.11418600000002</v>
       </c>
       <c r="E103" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.6435127999999963</v>
       </c>
       <c r="G103" t="s">
@@ -3313,11 +4836,31 @@
         <v>287.24724859999998</v>
       </c>
       <c r="I103" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3.6422048999999674</v>
       </c>
-    </row>
-    <row r="104" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K103" t="s">
+        <v>94</v>
+      </c>
+      <c r="L103">
+        <v>173.07956350000001</v>
+      </c>
+      <c r="M103" s="2">
+        <f t="shared" si="8"/>
+        <v>2.7563478000000146</v>
+      </c>
+      <c r="O103" t="s">
+        <v>94</v>
+      </c>
+      <c r="P103">
+        <v>187.0274455</v>
+      </c>
+      <c r="Q103" s="2">
+        <f t="shared" si="9"/>
+        <v>2.9321667000000105</v>
+      </c>
+    </row>
+    <row r="104" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C104" t="s">
         <v>95</v>
       </c>
@@ -3325,7 +4868,7 @@
         <v>368.91659499999997</v>
       </c>
       <c r="E104" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.8024089999999546</v>
       </c>
       <c r="G104" t="s">
@@ -3335,11 +4878,31 @@
         <v>293.5300742</v>
       </c>
       <c r="I104" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>6.2828256000000238</v>
       </c>
-    </row>
-    <row r="105" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K104" t="s">
+        <v>95</v>
+      </c>
+      <c r="L104">
+        <v>175.8527053</v>
+      </c>
+      <c r="M104" s="2">
+        <f t="shared" si="8"/>
+        <v>2.7731417999999906</v>
+      </c>
+      <c r="O104" t="s">
+        <v>95</v>
+      </c>
+      <c r="P104">
+        <v>190.68611300000001</v>
+      </c>
+      <c r="Q104" s="2">
+        <f t="shared" si="9"/>
+        <v>3.6586675000000071</v>
+      </c>
+    </row>
+    <row r="105" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C105" t="s">
         <v>96</v>
       </c>
@@ -3347,7 +4910,7 @@
         <v>373.82988920000003</v>
       </c>
       <c r="E105" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.9132942000000526</v>
       </c>
       <c r="G105" t="s">
@@ -3357,11 +4920,31 @@
         <v>297.4801946</v>
       </c>
       <c r="I105" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3.950120400000003</v>
       </c>
-    </row>
-    <row r="106" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K105" t="s">
+        <v>96</v>
+      </c>
+      <c r="L105">
+        <v>178.61445520000001</v>
+      </c>
+      <c r="M105" s="2">
+        <f t="shared" si="8"/>
+        <v>2.7617499000000123</v>
+      </c>
+      <c r="O105" t="s">
+        <v>96</v>
+      </c>
+      <c r="P105">
+        <v>193.78049010000001</v>
+      </c>
+      <c r="Q105" s="2">
+        <f t="shared" si="9"/>
+        <v>3.0943771000000027</v>
+      </c>
+    </row>
+    <row r="106" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C106" t="s">
         <v>97</v>
       </c>
@@ -3369,7 +4952,7 @@
         <v>378.61906260000001</v>
       </c>
       <c r="E106" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.7891733999999815</v>
       </c>
       <c r="G106" t="s">
@@ -3379,11 +4962,31 @@
         <v>301.35527589999998</v>
       </c>
       <c r="I106" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3.8750812999999766</v>
       </c>
-    </row>
-    <row r="107" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K106" t="s">
+        <v>97</v>
+      </c>
+      <c r="L106">
+        <v>181.44207399999999</v>
+      </c>
+      <c r="M106" s="2">
+        <f t="shared" si="8"/>
+        <v>2.827618799999982</v>
+      </c>
+      <c r="O106" t="s">
+        <v>97</v>
+      </c>
+      <c r="P106">
+        <v>196.7592502</v>
+      </c>
+      <c r="Q106" s="2">
+        <f t="shared" si="9"/>
+        <v>2.9787600999999881</v>
+      </c>
+    </row>
+    <row r="107" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C107" t="s">
         <v>98</v>
       </c>
@@ -3391,7 +4994,7 @@
         <v>382.78432930000002</v>
       </c>
       <c r="E107" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.1652667000000179</v>
       </c>
       <c r="G107" t="s">
@@ -3401,11 +5004,31 @@
         <v>304.78854009999998</v>
       </c>
       <c r="I107" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3.4332641999999964</v>
       </c>
-    </row>
-    <row r="108" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K107" t="s">
+        <v>98</v>
+      </c>
+      <c r="L107">
+        <v>184.2479438</v>
+      </c>
+      <c r="M107" s="2">
+        <f t="shared" si="8"/>
+        <v>2.8058698000000106</v>
+      </c>
+      <c r="O107" t="s">
+        <v>98</v>
+      </c>
+      <c r="P107">
+        <v>199.54673289999999</v>
+      </c>
+      <c r="Q107" s="2">
+        <f t="shared" si="9"/>
+        <v>2.7874826999999982</v>
+      </c>
+    </row>
+    <row r="108" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C108" t="s">
         <v>99</v>
       </c>
@@ -3413,7 +5036,7 @@
         <v>386.97344429999998</v>
       </c>
       <c r="E108" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.1891149999999584</v>
       </c>
       <c r="G108" t="s">
@@ -3423,11 +5046,31 @@
         <v>308.22358989999998</v>
       </c>
       <c r="I108" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3.4350498000000016</v>
       </c>
-    </row>
-    <row r="109" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K108" t="s">
+        <v>99</v>
+      </c>
+      <c r="L108">
+        <v>186.8559204</v>
+      </c>
+      <c r="M108" s="2">
+        <f t="shared" si="8"/>
+        <v>2.6079766000000006</v>
+      </c>
+      <c r="O108" t="s">
+        <v>99</v>
+      </c>
+      <c r="P108">
+        <v>202.25293959999999</v>
+      </c>
+      <c r="Q108" s="2">
+        <f t="shared" si="9"/>
+        <v>2.7062066999999956</v>
+      </c>
+    </row>
+    <row r="109" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C109" t="s">
         <v>19</v>
       </c>
@@ -3435,7 +5078,7 @@
         <v>387.0363643</v>
       </c>
       <c r="E109" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>6.2920000000019627E-2</v>
       </c>
       <c r="G109" t="s">
@@ -3445,11 +5088,31 @@
         <v>308.23073540000001</v>
       </c>
       <c r="I109" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>7.145500000035554E-3</v>
       </c>
-    </row>
-    <row r="111" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K109" t="s">
+        <v>19</v>
+      </c>
+      <c r="L109">
+        <v>186.861908</v>
+      </c>
+      <c r="M109" s="2">
+        <f t="shared" si="8"/>
+        <v>5.9875999999974283E-3</v>
+      </c>
+      <c r="O109" t="s">
+        <v>19</v>
+      </c>
+      <c r="P109">
+        <v>202.259896</v>
+      </c>
+      <c r="Q109" s="2">
+        <f t="shared" si="9"/>
+        <v>6.9564000000070791E-3</v>
+      </c>
+    </row>
+    <row r="111" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C111" s="1">
         <v>38.510790100000001</v>
       </c>
@@ -3457,7 +5120,7 @@
         <v>387.0363643</v>
       </c>
     </row>
-    <row r="112" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C112">
         <f>C111/4</f>
         <v>9.6276975250000003</v>
@@ -3467,9 +5130,108 @@
         <v>15.481454572000001</v>
       </c>
     </row>
+    <row r="114" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C114">
+        <v>4</v>
+      </c>
+      <c r="D114">
+        <v>39.462000000000003</v>
+      </c>
+      <c r="E114">
+        <f>D114/C114</f>
+        <v>9.8655000000000008</v>
+      </c>
+    </row>
+    <row r="115" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C115">
+        <v>9</v>
+      </c>
+      <c r="D115">
+        <v>75.350999999999999</v>
+      </c>
+      <c r="E115">
+        <f t="shared" ref="E115:E122" si="12">D115/C115</f>
+        <v>8.3723333333333336</v>
+      </c>
+    </row>
+    <row r="116" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C116">
+        <v>16</v>
+      </c>
+      <c r="D116">
+        <v>139.28100000000001</v>
+      </c>
+      <c r="E116">
+        <f t="shared" si="12"/>
+        <v>8.7050625000000004</v>
+      </c>
+    </row>
+    <row r="117" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C117">
+        <v>25</v>
+      </c>
+      <c r="D117">
+        <v>228</v>
+      </c>
+      <c r="E117">
+        <f t="shared" si="12"/>
+        <v>9.1199999999999992</v>
+      </c>
+    </row>
+    <row r="118" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C118">
+        <v>36</v>
+      </c>
+      <c r="D118">
+        <v>454</v>
+      </c>
+      <c r="E118">
+        <f t="shared" si="12"/>
+        <v>12.611111111111111</v>
+      </c>
+    </row>
+    <row r="119" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C119">
+        <v>49</v>
+      </c>
+      <c r="E119">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C120">
+        <v>64</v>
+      </c>
+      <c r="E120">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F120" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="121" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C121">
+        <v>81</v>
+      </c>
+      <c r="E121">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C122">
+        <v>100</v>
+      </c>
+      <c r="E122">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="E3:E21">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3481,7 +5243,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I21">
-    <cfRule type="colorScale" priority="9">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3493,7 +5255,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:M21">
-    <cfRule type="colorScale" priority="11">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3505,6 +5267,42 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3:Q21">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27:E109">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I27:I109">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M27:M109">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -3516,7 +5314,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E27:E109">
+  <conditionalFormatting sqref="Q27:Q82">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3528,7 +5326,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I27:I109">
+  <conditionalFormatting sqref="Q83:Q109">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Full generation run, screenshots broken
</commit_message>
<xml_diff>
--- a/Test Results.xlsx
+++ b/Test Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Marshall\Documents\GitHub\Column-Sort---Current\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Documents\RevitUtilities-master\RevitUtilities-master\Column Sort - Current\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A49505E-B8A9-4F94-87C5-DB30987BC3E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95627CE9-CDFC-4960-ABA9-5A255B23E4D5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B6784F4F-6013-4AC1-BB34-1B8804D31140}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6784F4F-6013-4AC1-BB34-1B8804D31140}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -2008,6 +2006,732 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Score</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$341:$L$341</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$351:$L$351</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1530.6964519819876</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1524.7074149217453</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2155.362694210231</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1336.1080340053368</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1609.1746991503287</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1365.8869160415868</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1328.9095788424991</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1331.3374793925934</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1367.4430680111645</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1409.2488704528241</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1298.1360623689534</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8E99-4FBB-A5F2-AA443F17E671}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1549523984"/>
+        <c:axId val="1521818000"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1549523984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1521818000"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1521818000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1549523984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Standard</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Deviation</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$341:$L$341</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$352:$L$352</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>46.198995030515412</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36.701716100254245</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.337116987129807</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31.764331078629471</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>237.9143175495544</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41.3793813269629</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>51.97230864416148</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27.321387180225031</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.342186551633752</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>49.425850069475864</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>34.345698094909764</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B89E-44B3-BFEB-4F81EFF300EE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1515923008"/>
+        <c:axId val="1526487840"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1515923008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1526487840"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1526487840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1515923008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2168,6 +2892,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3717,6 +4521,1038 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4373,6 +6209,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>370251</xdr:colOff>
+      <xdr:row>356</xdr:row>
+      <xdr:rowOff>103575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>818602</xdr:colOff>
+      <xdr:row>370</xdr:row>
+      <xdr:rowOff>121459</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4850D18-C110-4072-ABC8-8865D073A762}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>924486</xdr:colOff>
+      <xdr:row>356</xdr:row>
+      <xdr:rowOff>68355</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>252133</xdr:colOff>
+      <xdr:row>370</xdr:row>
+      <xdr:rowOff>144555</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B99E2696-FF74-4AAF-8281-22DA797EDFDF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4678,10 +6586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B55F16F4-02C8-43F7-AF82-ACA786E304B0}">
-  <dimension ref="A1:V313"/>
+  <dimension ref="A1:V352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A290" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="M318" sqref="M318"/>
+    <sheetView tabSelected="1" topLeftCell="A331" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N365" sqref="N365"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12449,6 +14357,448 @@
       <c r="H313">
         <f t="shared" si="14"/>
         <v>47.401396880036714</v>
+      </c>
+    </row>
+    <row r="341" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B341">
+        <v>10</v>
+      </c>
+      <c r="C341">
+        <v>20</v>
+      </c>
+      <c r="D341">
+        <v>30</v>
+      </c>
+      <c r="E341">
+        <v>40</v>
+      </c>
+      <c r="F341">
+        <v>50</v>
+      </c>
+      <c r="G341">
+        <v>60</v>
+      </c>
+      <c r="H341">
+        <v>70</v>
+      </c>
+      <c r="I341">
+        <v>80</v>
+      </c>
+      <c r="J341">
+        <v>90</v>
+      </c>
+      <c r="K341">
+        <v>100</v>
+      </c>
+      <c r="L341">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="342" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B342" s="2">
+        <v>1465.5186431346799</v>
+      </c>
+      <c r="C342" s="2">
+        <v>1435.8069565900701</v>
+      </c>
+      <c r="D342" s="2">
+        <v>2115.08873266926</v>
+      </c>
+      <c r="E342" s="2">
+        <v>1293.02879231164</v>
+      </c>
+      <c r="F342" s="2">
+        <v>1429.0004056185501</v>
+      </c>
+      <c r="G342" s="2">
+        <v>1298.65171650354</v>
+      </c>
+      <c r="H342" s="2">
+        <v>1222.8486683265</v>
+      </c>
+      <c r="I342" s="2">
+        <v>1284.08368350764</v>
+      </c>
+      <c r="J342" s="2">
+        <v>1341.45550443758</v>
+      </c>
+      <c r="K342" s="2">
+        <v>1315.6598868884</v>
+      </c>
+      <c r="L342" s="2">
+        <v>1248.5529618794999</v>
+      </c>
+    </row>
+    <row r="343" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B343" s="2">
+        <v>1472.1486459443099</v>
+      </c>
+      <c r="C343" s="2">
+        <v>1515.8069565900701</v>
+      </c>
+      <c r="D343" s="2">
+        <v>2134.85923592981</v>
+      </c>
+      <c r="E343" s="2">
+        <v>1293.02879231164</v>
+      </c>
+      <c r="F343" s="2">
+        <v>1429.0004056185501</v>
+      </c>
+      <c r="G343" s="2">
+        <v>1338.65171650354</v>
+      </c>
+      <c r="H343" s="2">
+        <v>1271.85329235176</v>
+      </c>
+      <c r="I343" s="2">
+        <v>1305.6584651579799</v>
+      </c>
+      <c r="J343" s="2">
+        <v>1346.6000769667201</v>
+      </c>
+      <c r="K343" s="2">
+        <v>1383.93533669368</v>
+      </c>
+      <c r="L343" s="2">
+        <v>1270.73624713759</v>
+      </c>
+    </row>
+    <row r="344" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B344" s="2">
+        <v>1486.8064484910401</v>
+      </c>
+      <c r="C344" s="2">
+        <v>1515.8069565900701</v>
+      </c>
+      <c r="D344" s="2">
+        <v>2135.1980678023301</v>
+      </c>
+      <c r="E344" s="2">
+        <v>1311.0542152052601</v>
+      </c>
+      <c r="F344" s="2">
+        <v>1441.7315765421399</v>
+      </c>
+      <c r="G344" s="2">
+        <v>1338.65171650354</v>
+      </c>
+      <c r="H344" s="2">
+        <v>1303.8233365577901</v>
+      </c>
+      <c r="I344" s="2">
+        <v>1319.0831398625501</v>
+      </c>
+      <c r="J344" s="2">
+        <v>1348.2594119220601</v>
+      </c>
+      <c r="K344" s="2">
+        <v>1383.93533669368</v>
+      </c>
+      <c r="L344" s="2">
+        <v>1270.73624713759</v>
+      </c>
+    </row>
+    <row r="345" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B345" s="2">
+        <v>1527.5291081391699</v>
+      </c>
+      <c r="C345" s="2">
+        <v>1515.8402250547299</v>
+      </c>
+      <c r="D345" s="2">
+        <v>2155.08873266925</v>
+      </c>
+      <c r="E345" s="2">
+        <v>1330.7478769977199</v>
+      </c>
+      <c r="F345" s="2">
+        <v>1469.0004056185501</v>
+      </c>
+      <c r="G345" s="2">
+        <v>1338.65171650354</v>
+      </c>
+      <c r="H345" s="2">
+        <v>1333.6562571931199</v>
+      </c>
+      <c r="I345" s="2">
+        <v>1326.90170500719</v>
+      </c>
+      <c r="J345" s="2">
+        <v>1374.36811621017</v>
+      </c>
+      <c r="K345" s="2">
+        <v>1397.2695105543701</v>
+      </c>
+      <c r="L345" s="2">
+        <v>1270.73624713759</v>
+      </c>
+    </row>
+    <row r="346" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B346" s="2">
+        <v>1533.55018177585</v>
+      </c>
+      <c r="C346" s="2">
+        <v>1535.4341298802999</v>
+      </c>
+      <c r="D346" s="2">
+        <v>2155.08873266925</v>
+      </c>
+      <c r="E346" s="2">
+        <v>1332.18297183964</v>
+      </c>
+      <c r="F346" s="2">
+        <v>1602.97765242886</v>
+      </c>
+      <c r="G346" s="2">
+        <v>1360.3593763014001</v>
+      </c>
+      <c r="H346" s="2">
+        <v>1338.2396253628899</v>
+      </c>
+      <c r="I346" s="2">
+        <v>1327.7665865252</v>
+      </c>
+      <c r="J346" s="2">
+        <v>1374.36811621017</v>
+      </c>
+      <c r="K346" s="2">
+        <v>1403.91090035604</v>
+      </c>
+      <c r="L346" s="2">
+        <v>1295.6203021629899</v>
+      </c>
+    </row>
+    <row r="347" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B347" s="2">
+        <v>1545.5186431346799</v>
+      </c>
+      <c r="C347" s="2">
+        <v>1535.4341298802999</v>
+      </c>
+      <c r="D347" s="2">
+        <v>2155.08873266926</v>
+      </c>
+      <c r="E347" s="2">
+        <v>1351.0542152052601</v>
+      </c>
+      <c r="F347" s="2">
+        <v>1602.97765242886</v>
+      </c>
+      <c r="G347" s="2">
+        <v>1378.65171650354</v>
+      </c>
+      <c r="H347" s="2">
+        <v>1342.8486683265</v>
+      </c>
+      <c r="I347" s="2">
+        <v>1334.8866549781901</v>
+      </c>
+      <c r="J347" s="2">
+        <v>1374.36811621017</v>
+      </c>
+      <c r="K347" s="2">
+        <v>1403.91090035604</v>
+      </c>
+      <c r="L347" s="2">
+        <v>1310.73624713759</v>
+      </c>
+    </row>
+    <row r="348" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B348" s="2">
+        <v>1552.1486459443099</v>
+      </c>
+      <c r="C348" s="2">
+        <v>1536.21521156005</v>
+      </c>
+      <c r="D348" s="2">
+        <v>2174.85923592981</v>
+      </c>
+      <c r="E348" s="2">
+        <v>1352.0733499738801</v>
+      </c>
+      <c r="F348" s="2">
+        <v>1615.27757069263</v>
+      </c>
+      <c r="G348" s="2">
+        <v>1380.3565867039299</v>
+      </c>
+      <c r="H348" s="2">
+        <v>1372.2058106582299</v>
+      </c>
+      <c r="I348" s="2">
+        <v>1345.6584651579799</v>
+      </c>
+      <c r="J348" s="2">
+        <v>1374.36811621017</v>
+      </c>
+      <c r="K348" s="2">
+        <v>1444.01631630304</v>
+      </c>
+      <c r="L348" s="2">
+        <v>1317.8851288799401</v>
+      </c>
+    </row>
+    <row r="349" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B349" s="2">
+        <v>1585.5186431346799</v>
+      </c>
+      <c r="C349" s="2">
+        <v>1555.8069565900701</v>
+      </c>
+      <c r="D349" s="2">
+        <v>2178.3220647338999</v>
+      </c>
+      <c r="E349" s="2">
+        <v>1370.7478769977199</v>
+      </c>
+      <c r="F349" s="2">
+        <v>1655.27757069263</v>
+      </c>
+      <c r="G349" s="2">
+        <v>1420.3565867039299</v>
+      </c>
+      <c r="H349" s="2">
+        <v>1378.2396253628899</v>
+      </c>
+      <c r="I349" s="2">
+        <v>1351.84295632617</v>
+      </c>
+      <c r="J349" s="2">
+        <v>1386.6000769667201</v>
+      </c>
+      <c r="K349" s="2">
+        <v>1445.2109995578401</v>
+      </c>
+      <c r="L349" s="2">
+        <v>1340.33605096785</v>
+      </c>
+    </row>
+    <row r="350" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B350" s="2">
+        <v>1607.5291081391699</v>
+      </c>
+      <c r="C350" s="2">
+        <v>1576.21521156005</v>
+      </c>
+      <c r="D350" s="2">
+        <v>2194.6707128192102</v>
+      </c>
+      <c r="E350" s="2">
+        <v>1391.0542152052701</v>
+      </c>
+      <c r="F350" s="2">
+        <v>2237.3290527121899</v>
+      </c>
+      <c r="G350" s="2">
+        <v>1438.65111214732</v>
+      </c>
+      <c r="H350" s="2">
+        <v>1396.4709254428101</v>
+      </c>
+      <c r="I350" s="2">
+        <v>1386.15565801044</v>
+      </c>
+      <c r="J350" s="2">
+        <v>1386.6000769667201</v>
+      </c>
+      <c r="K350" s="2">
+        <v>1505.3906466723299</v>
+      </c>
+      <c r="L350" s="2">
+        <v>1357.8851288799401</v>
+      </c>
+    </row>
+    <row r="351" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B351" s="2">
+        <f>AVERAGE(B342:B350)</f>
+        <v>1530.6964519819876</v>
+      </c>
+      <c r="C351" s="2">
+        <f t="shared" ref="C351:L351" si="15">AVERAGE(C342:C350)</f>
+        <v>1524.7074149217453</v>
+      </c>
+      <c r="D351" s="2">
+        <f t="shared" si="15"/>
+        <v>2155.362694210231</v>
+      </c>
+      <c r="E351" s="2">
+        <f t="shared" si="15"/>
+        <v>1336.1080340053368</v>
+      </c>
+      <c r="F351" s="2">
+        <f t="shared" si="15"/>
+        <v>1609.1746991503287</v>
+      </c>
+      <c r="G351" s="2">
+        <f t="shared" si="15"/>
+        <v>1365.8869160415868</v>
+      </c>
+      <c r="H351" s="2">
+        <f t="shared" si="15"/>
+        <v>1328.9095788424991</v>
+      </c>
+      <c r="I351" s="2">
+        <f t="shared" si="15"/>
+        <v>1331.3374793925934</v>
+      </c>
+      <c r="J351" s="2">
+        <f t="shared" si="15"/>
+        <v>1367.4430680111645</v>
+      </c>
+      <c r="K351" s="2">
+        <f t="shared" si="15"/>
+        <v>1409.2488704528241</v>
+      </c>
+      <c r="L351" s="2">
+        <f t="shared" si="15"/>
+        <v>1298.1360623689534</v>
+      </c>
+    </row>
+    <row r="352" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B352" s="2">
+        <f>_xlfn.STDEV.P(B342:B350)</f>
+        <v>46.198995030515412</v>
+      </c>
+      <c r="C352" s="2">
+        <f t="shared" ref="C352:L352" si="16">_xlfn.STDEV.P(C342:C350)</f>
+        <v>36.701716100254245</v>
+      </c>
+      <c r="D352" s="2">
+        <f t="shared" si="16"/>
+        <v>23.337116987129807</v>
+      </c>
+      <c r="E352" s="2">
+        <f t="shared" si="16"/>
+        <v>31.764331078629471</v>
+      </c>
+      <c r="F352" s="2">
+        <f t="shared" si="16"/>
+        <v>237.9143175495544</v>
+      </c>
+      <c r="G352" s="2">
+        <f t="shared" si="16"/>
+        <v>41.3793813269629</v>
+      </c>
+      <c r="H352" s="2">
+        <f t="shared" si="16"/>
+        <v>51.97230864416148</v>
+      </c>
+      <c r="I352" s="2">
+        <f t="shared" si="16"/>
+        <v>27.321387180225031</v>
+      </c>
+      <c r="J352" s="2">
+        <f t="shared" si="16"/>
+        <v>16.342186551633752</v>
+      </c>
+      <c r="K352" s="2">
+        <f t="shared" si="16"/>
+        <v>49.425850069475864</v>
+      </c>
+      <c r="L352" s="2">
+        <f t="shared" si="16"/>
+        <v>34.345698094909764</v>
       </c>
     </row>
   </sheetData>

</xml_diff>